<commit_message>
Published state of ETDataset on 19 August 2016
</commit_message>
<xml_diff>
--- a/carriers_source_analyses/bio_lng.carrier.xlsx
+++ b/carriers_source_analyses/bio_lng.carrier.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="-20" windowWidth="19200" windowHeight="23460" tabRatio="762" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16100" tabRatio="762" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="190">
   <si>
     <t>Source</t>
   </si>
@@ -599,28 +599,117 @@
   <si>
     <t>http://refman.et-model.com/publications/1996</t>
   </si>
+  <si>
+    <t>potential_co2_conversion_per_mj</t>
+  </si>
+  <si>
+    <t>Actual CO2 emission from biomass</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>potential_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>co2_conversion_per_mj</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>potential_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>co2_conversion_per_mj</t>
+    </r>
+  </si>
+  <si>
+    <t>IPCC</t>
+  </si>
+  <si>
+    <t>global</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>http://refman.et-model.com/publications/1710</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IPCC_2006_Guidelines for National Greenhouse Gas Inventories - Vol 2 Energy - Ch 1 Introduction.pdf</t>
+  </si>
+  <si>
+    <t>kg CO2/TJ</t>
+  </si>
+  <si>
+    <t>TJ/MJ</t>
+  </si>
+  <si>
+    <t>gas biomass</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="9">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;_-* #,##0.00\-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.000000000"/>
-    <numFmt numFmtId="168" formatCode="0.0000000000"/>
-    <numFmt numFmtId="169" formatCode="0.0%"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="0.00000000000000"/>
+  <numFmts count="10">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;_-* #,##0.00\-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.000000000"/>
+    <numFmt numFmtId="169" formatCode="0.0000000000"/>
+    <numFmt numFmtId="170" formatCode="0.0%"/>
+    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="172" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="173" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Lettertype hoofdtekst"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -837,6 +926,26 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF474747"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Lettertype hoofdtekst"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1266,630 +1375,655 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="336">
+  <cellStyleXfs count="337">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="206">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="18" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="183" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="167" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="183" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="168" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="25" fillId="0" borderId="0" xfId="320" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="27" fillId="0" borderId="0" xfId="320" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="29" fillId="0" borderId="0" xfId="320" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" xfId="320" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="25" fillId="0" borderId="0" xfId="321" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="29" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="25" fillId="0" borderId="0" xfId="320" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="27" fillId="0" borderId="0" xfId="321" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="320" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="172" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="27" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="171" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="35" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="25" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="173" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="2" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="33" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="1" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="336">
+  <cellStyles count="337">
     <cellStyle name="Comma" xfId="320" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2135,6 +2269,7 @@
     <cellStyle name="Followed Hyperlink" xfId="333" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="335" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2891,6 +3026,44 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>220</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>258</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7874000" y="114655600"/>
+          <a:ext cx="9779000" cy="8293100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3559,9 +3732,11 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:K15"/>
+  <dimension ref="B1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -3585,28 +3760,28 @@
       <c r="G1" s="33"/>
     </row>
     <row r="2" spans="2:11" ht="15" customHeight="1">
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="194" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="178"/>
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="196"/>
       <c r="F2" s="33"/>
       <c r="G2" s="33"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="179"/>
-      <c r="C3" s="180"/>
-      <c r="D3" s="180"/>
-      <c r="E3" s="181"/>
+      <c r="B3" s="197"/>
+      <c r="C3" s="198"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="199"/>
       <c r="F3" s="33"/>
       <c r="G3" s="33"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="182"/>
-      <c r="C4" s="183"/>
-      <c r="D4" s="183"/>
-      <c r="E4" s="184"/>
+      <c r="B4" s="200"/>
+      <c r="C4" s="201"/>
+      <c r="D4" s="201"/>
+      <c r="E4" s="202"/>
       <c r="F4" s="33"/>
       <c r="G4" s="33"/>
     </row>
@@ -3753,37 +3928,59 @@
       </c>
       <c r="J13" s="43"/>
     </row>
-    <row r="14" spans="2:11" ht="16" thickBot="1">
-      <c r="B14" s="38"/>
-      <c r="C14" s="34" t="s">
+    <row r="14" spans="2:11" s="42" customFormat="1" ht="19" thickBot="1">
+      <c r="B14" s="23"/>
+      <c r="C14" s="177" t="s">
+        <v>178</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="191">
+        <f>'Research data'!G10</f>
+        <v>5.4600000000000003E-2</v>
+      </c>
+      <c r="F14" s="177"/>
+      <c r="G14" s="177" t="s">
+        <v>179</v>
+      </c>
+      <c r="H14" s="30"/>
+      <c r="I14" s="205" t="s">
+        <v>182</v>
+      </c>
+      <c r="J14" s="43"/>
+    </row>
+    <row r="15" spans="2:11" ht="16" thickBot="1">
+      <c r="B15" s="38"/>
+      <c r="C15" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D15" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="108">
-        <f>'Research data'!G10</f>
+      <c r="E15" s="108">
+        <f>'Research data'!G11</f>
         <v>15279471.503999995</v>
       </c>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="121" t="s">
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="J14" s="95"/>
-      <c r="K14" s="33"/>
-    </row>
-    <row r="15" spans="2:11" ht="20" customHeight="1" thickBot="1">
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="41"/>
+      <c r="J15" s="95"/>
+      <c r="K15" s="33"/>
+    </row>
+    <row r="16" spans="2:11" ht="20" customHeight="1" thickBot="1">
+      <c r="B16" s="39"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3836,10 +4033,10 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0">
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B1:Q12"/>
+  <dimension ref="B1:R13"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3858,14 +4055,14 @@
     <col min="12" max="12" width="3.125" style="67" customWidth="1"/>
     <col min="13" max="13" width="12.875" style="67" customWidth="1"/>
     <col min="14" max="14" width="2.625" style="67" customWidth="1"/>
-    <col min="15" max="15" width="8.5" style="67" customWidth="1"/>
-    <col min="16" max="16" width="2.625" style="67" customWidth="1"/>
-    <col min="17" max="17" width="60" style="66" customWidth="1"/>
-    <col min="18" max="16384" width="10.625" style="66"/>
+    <col min="15" max="16" width="8.5" style="67" customWidth="1"/>
+    <col min="17" max="17" width="2.625" style="67" customWidth="1"/>
+    <col min="18" max="18" width="60" style="66" customWidth="1"/>
+    <col min="19" max="16384" width="10.625" style="66"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="16" thickBot="1"/>
-    <row r="2" spans="2:17">
+    <row r="1" spans="2:18" ht="16" thickBot="1"/>
+    <row r="2" spans="2:18">
       <c r="B2" s="68"/>
       <c r="C2" s="69"/>
       <c r="D2" s="69"/>
@@ -3881,9 +4078,10 @@
       <c r="N2" s="70"/>
       <c r="O2" s="70"/>
       <c r="P2" s="70"/>
-      <c r="Q2" s="71"/>
-    </row>
-    <row r="3" spans="2:17" s="24" customFormat="1">
+      <c r="Q2" s="70"/>
+      <c r="R2" s="71"/>
+    </row>
+    <row r="3" spans="2:18" s="24" customFormat="1">
       <c r="B3" s="23"/>
       <c r="C3" s="99" t="s">
         <v>29</v>
@@ -3912,12 +4110,15 @@
       <c r="O3" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="1" t="s">
+      <c r="P3" s="64" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:17">
+    <row r="4" spans="2:18">
       <c r="B4" s="72"/>
       <c r="C4" s="73"/>
       <c r="D4" s="73"/>
@@ -3932,10 +4133,11 @@
       <c r="M4" s="96"/>
       <c r="N4" s="98"/>
       <c r="O4" s="96"/>
-      <c r="P4" s="98"/>
-      <c r="Q4" s="2"/>
-    </row>
-    <row r="5" spans="2:17" ht="16" thickBot="1">
+      <c r="P4" s="96"/>
+      <c r="Q4" s="98"/>
+      <c r="R4" s="2"/>
+    </row>
+    <row r="5" spans="2:18" ht="16" thickBot="1">
       <c r="B5" s="72"/>
       <c r="C5" s="18" t="s">
         <v>48</v>
@@ -3953,9 +4155,10 @@
       <c r="N5" s="16"/>
       <c r="O5" s="16"/>
       <c r="P5" s="16"/>
-      <c r="Q5" s="3"/>
-    </row>
-    <row r="6" spans="2:17" ht="16" thickBot="1">
+      <c r="Q5" s="16"/>
+      <c r="R5" s="3"/>
+    </row>
+    <row r="6" spans="2:18" ht="16" thickBot="1">
       <c r="B6" s="72"/>
       <c r="C6" s="109" t="s">
         <v>35</v>
@@ -3981,9 +4184,10 @@
       <c r="N6" s="17"/>
       <c r="O6" s="16"/>
       <c r="P6" s="16"/>
-      <c r="Q6" s="3"/>
-    </row>
-    <row r="7" spans="2:17" s="6" customFormat="1" ht="16" thickBot="1">
+      <c r="Q6" s="16"/>
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="2:18" s="6" customFormat="1" ht="16" thickBot="1">
       <c r="B7" s="5"/>
       <c r="C7" s="110" t="s">
         <v>36</v>
@@ -4011,9 +4215,10 @@
       <c r="N7" s="17"/>
       <c r="O7" s="16"/>
       <c r="P7" s="16"/>
-      <c r="Q7" s="158"/>
-    </row>
-    <row r="8" spans="2:17" s="6" customFormat="1" ht="16" thickBot="1">
+      <c r="Q7" s="16"/>
+      <c r="R7" s="158"/>
+    </row>
+    <row r="8" spans="2:18" s="6" customFormat="1" ht="16" thickBot="1">
       <c r="B8" s="5"/>
       <c r="C8" s="110" t="s">
         <v>149</v>
@@ -4043,9 +4248,10 @@
       <c r="N8" s="17"/>
       <c r="O8" s="16"/>
       <c r="P8" s="16"/>
-      <c r="Q8" s="149"/>
-    </row>
-    <row r="9" spans="2:17" s="6" customFormat="1" ht="16" thickBot="1">
+      <c r="Q8" s="16"/>
+      <c r="R8" s="149"/>
+    </row>
+    <row r="9" spans="2:18" s="6" customFormat="1" ht="16" thickBot="1">
       <c r="B9" s="5"/>
       <c r="C9" s="111" t="s">
         <v>37</v>
@@ -4071,48 +4277,48 @@
       <c r="N9" s="17"/>
       <c r="O9" s="16"/>
       <c r="P9" s="16"/>
-      <c r="Q9" s="173" t="s">
+      <c r="Q9" s="16"/>
+      <c r="R9" s="173" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="2:17" ht="16" thickBot="1">
-      <c r="B10" s="72"/>
-      <c r="C10" s="111" t="s">
-        <v>38</v>
+    <row r="10" spans="2:18" s="6" customFormat="1" ht="16" thickBot="1">
+      <c r="B10" s="5"/>
+      <c r="C10" s="178" t="s">
+        <v>180</v>
       </c>
       <c r="D10" s="111" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" s="111" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="44">
-        <f>K10</f>
-        <v>15279471.503999995</v>
-      </c>
-      <c r="H10" s="76"/>
+        <v>43</v>
+      </c>
+      <c r="G10" s="190">
+        <f>P10</f>
+        <v>5.4600000000000003E-2</v>
+      </c>
+      <c r="H10" s="4"/>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
-      <c r="K10" s="44">
-        <f>Notes!H39</f>
-        <v>15279471.503999995</v>
-      </c>
+      <c r="K10" s="17"/>
       <c r="L10" s="17"/>
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
       <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="149" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17" ht="16" thickBot="1">
+      <c r="P10" s="203">
+        <f>Notes!G251</f>
+        <v>5.4600000000000003E-2</v>
+      </c>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="173"/>
+    </row>
+    <row r="11" spans="2:18" ht="16" thickBot="1">
       <c r="B11" s="72"/>
-      <c r="C11" s="159" t="s">
-        <v>158</v>
+      <c r="C11" s="111" t="s">
+        <v>38</v>
       </c>
       <c r="D11" s="111" t="s">
         <v>38</v>
@@ -4121,28 +4327,33 @@
         <v>38</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="G11" s="44">
-        <f>I11</f>
-        <v>20.7</v>
+        <f>K11</f>
+        <v>15279471.503999995</v>
       </c>
       <c r="H11" s="76"/>
-      <c r="I11" s="45">
-        <f>Notes!E169</f>
-        <v>20.7</v>
-      </c>
+      <c r="I11" s="17"/>
       <c r="J11" s="17"/>
+      <c r="K11" s="44">
+        <f>Notes!H39</f>
+        <v>15279471.503999995</v>
+      </c>
       <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
       <c r="N11" s="17"/>
       <c r="O11" s="16"/>
       <c r="P11" s="16"/>
-      <c r="Q11" s="149"/>
-    </row>
-    <row r="12" spans="2:17" ht="16" thickBot="1">
+      <c r="Q11" s="16"/>
+      <c r="R11" s="149" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" ht="16" thickBot="1">
       <c r="B12" s="72"/>
       <c r="C12" s="159" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D12" s="111" t="s">
         <v>38</v>
@@ -4151,21 +4362,53 @@
         <v>38</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="G12" s="44">
         <f>I12</f>
-        <v>0.41799999999999998</v>
+        <v>20.7</v>
       </c>
       <c r="H12" s="76"/>
       <c r="I12" s="45">
-        <f>Notes!E168</f>
-        <v>0.41799999999999998</v>
+        <f>Notes!E169</f>
+        <v>20.7</v>
       </c>
       <c r="J12" s="17"/>
       <c r="L12" s="17"/>
       <c r="N12" s="17"/>
       <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="149"/>
+    </row>
+    <row r="13" spans="2:18" ht="16" thickBot="1">
+      <c r="B13" s="72"/>
+      <c r="C13" s="159" t="s">
+        <v>161</v>
+      </c>
+      <c r="D13" s="111" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="111" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="44">
+        <f>I13</f>
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="H13" s="76"/>
+      <c r="I13" s="45">
+        <f>Notes!E168</f>
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="J13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4183,10 +4426,10 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0">
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B1:L14"/>
+  <dimension ref="B1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="33.125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4312,7 +4555,7 @@
       <c r="J7" s="55" t="s">
         <v>175</v>
       </c>
-      <c r="K7" s="185" t="s">
+      <c r="K7" s="176" t="s">
         <v>177</v>
       </c>
       <c r="L7" s="55" t="s">
@@ -4415,6 +4658,29 @@
       <c r="L14" s="55" t="s">
         <v>166</v>
       </c>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" s="51"/>
+      <c r="C15" s="179" t="s">
+        <v>181</v>
+      </c>
+      <c r="D15" s="60"/>
+      <c r="E15" s="180" t="s">
+        <v>182</v>
+      </c>
+      <c r="F15" s="180"/>
+      <c r="G15" s="54" t="s">
+        <v>183</v>
+      </c>
+      <c r="H15" s="55" t="s">
+        <v>184</v>
+      </c>
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="204" t="s">
+        <v>185</v>
+      </c>
+      <c r="L15" s="65"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4431,8 +4697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ697"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView topLeftCell="A185" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="D221" sqref="D221:J233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10286,7 +10552,7 @@
       <c r="Y208" s="112"/>
       <c r="Z208" s="112"/>
     </row>
-    <row r="209" spans="1:26" customFormat="1" ht="16">
+    <row r="209" spans="2:35" customFormat="1" ht="16">
       <c r="B209" s="102"/>
       <c r="C209" s="112"/>
       <c r="D209" s="112"/>
@@ -10313,7 +10579,7 @@
       <c r="Y209" s="112"/>
       <c r="Z209" s="112"/>
     </row>
-    <row r="210" spans="1:26" customFormat="1" ht="16">
+    <row r="210" spans="2:35" customFormat="1" ht="16">
       <c r="B210" s="102"/>
       <c r="C210" s="112"/>
       <c r="D210" s="112"/>
@@ -10340,7 +10606,7 @@
       <c r="Y210" s="112"/>
       <c r="Z210" s="112"/>
     </row>
-    <row r="211" spans="1:26" customFormat="1" ht="16">
+    <row r="211" spans="2:35" customFormat="1" ht="16">
       <c r="B211" s="102"/>
       <c r="C211" s="112"/>
       <c r="D211" s="112"/>
@@ -10367,7 +10633,7 @@
       <c r="Y211" s="112"/>
       <c r="Z211" s="112"/>
     </row>
-    <row r="212" spans="1:26" customFormat="1" ht="16">
+    <row r="212" spans="2:35" customFormat="1" ht="16">
       <c r="B212" s="102"/>
       <c r="C212" s="112"/>
       <c r="D212" s="112"/>
@@ -10394,7 +10660,7 @@
       <c r="Y212" s="112"/>
       <c r="Z212" s="112"/>
     </row>
-    <row r="213" spans="1:26" customFormat="1" ht="16">
+    <row r="213" spans="2:35" customFormat="1" ht="16">
       <c r="B213" s="102"/>
       <c r="C213" s="112"/>
       <c r="D213" s="112"/>
@@ -10421,7 +10687,7 @@
       <c r="Y213" s="112"/>
       <c r="Z213" s="112"/>
     </row>
-    <row r="214" spans="1:26" customFormat="1" ht="16">
+    <row r="214" spans="2:35" customFormat="1" ht="16">
       <c r="B214" s="102"/>
       <c r="C214" s="112"/>
       <c r="D214" s="112"/>
@@ -10448,7 +10714,7 @@
       <c r="Y214" s="112"/>
       <c r="Z214" s="112"/>
     </row>
-    <row r="215" spans="1:26" customFormat="1" ht="16">
+    <row r="215" spans="2:35" customFormat="1" ht="17" thickBot="1">
       <c r="B215" s="102"/>
       <c r="C215" s="112"/>
       <c r="D215" s="112"/>
@@ -10475,975 +10741,1759 @@
       <c r="Y215" s="112"/>
       <c r="Z215" s="112"/>
     </row>
-    <row r="216" spans="1:26" customFormat="1" ht="16">
-      <c r="A216" s="101"/>
-      <c r="B216" s="101"/>
-      <c r="C216" s="101"/>
-      <c r="D216" s="101"/>
-      <c r="E216" s="101"/>
-      <c r="F216" s="101"/>
-      <c r="G216" s="101"/>
-      <c r="H216" s="101"/>
-      <c r="I216" s="101"/>
-      <c r="J216" s="101"/>
-      <c r="K216" s="101"/>
-      <c r="L216" s="101"/>
-      <c r="M216" s="101"/>
-      <c r="N216" s="101"/>
-      <c r="O216" s="101"/>
-      <c r="P216" s="101"/>
-      <c r="Q216" s="101"/>
-      <c r="R216" s="101"/>
-      <c r="S216" s="101"/>
-      <c r="T216" s="112"/>
-      <c r="U216" s="112"/>
-      <c r="V216" s="112"/>
-      <c r="W216" s="112"/>
-      <c r="X216" s="112"/>
-      <c r="Y216" s="112"/>
-      <c r="Z216" s="112"/>
-    </row>
-    <row r="217" spans="1:26" customFormat="1" ht="17" thickBot="1">
-      <c r="A217" s="101"/>
-      <c r="B217" s="101"/>
-      <c r="C217" s="101"/>
-      <c r="D217" s="101"/>
-      <c r="E217" s="101"/>
-      <c r="F217" s="101"/>
-      <c r="G217" s="101"/>
-      <c r="H217" s="101"/>
-      <c r="I217" s="101"/>
-      <c r="J217" s="101"/>
-      <c r="K217" s="101"/>
-      <c r="L217" s="101"/>
-      <c r="M217" s="101"/>
-      <c r="N217" s="101"/>
-      <c r="O217" s="101"/>
-      <c r="P217" s="101"/>
-      <c r="Q217" s="101"/>
-      <c r="R217" s="101"/>
-      <c r="S217" s="101"/>
-      <c r="T217" s="112"/>
-      <c r="U217" s="112"/>
-      <c r="V217" s="112"/>
-      <c r="W217" s="112"/>
-      <c r="X217" s="112"/>
-      <c r="Y217" s="112"/>
-    </row>
-    <row r="218" spans="1:26" customFormat="1" ht="16">
-      <c r="A218" s="101"/>
-      <c r="B218" s="101"/>
-      <c r="C218" s="101"/>
-      <c r="D218" s="101"/>
-      <c r="E218" s="101"/>
-      <c r="F218" s="101"/>
-      <c r="G218" s="101"/>
-      <c r="H218" s="101"/>
-      <c r="I218" s="101"/>
-      <c r="J218" s="101"/>
-      <c r="K218" s="101"/>
-      <c r="L218" s="101"/>
-      <c r="M218" s="101"/>
-      <c r="N218" s="101"/>
-      <c r="O218" s="101"/>
-      <c r="P218" s="101"/>
-      <c r="Q218" s="101"/>
-      <c r="R218" s="101"/>
-      <c r="S218" s="101"/>
-      <c r="T218" s="105"/>
-      <c r="U218" s="24"/>
-      <c r="V218" s="24"/>
-      <c r="W218" s="24"/>
-      <c r="X218" s="24"/>
-      <c r="Y218" s="24"/>
-    </row>
-    <row r="219" spans="1:26" s="24" customFormat="1" ht="16">
+    <row r="216" spans="2:35" s="181" customFormat="1">
+      <c r="B216" s="182"/>
+      <c r="C216" s="183" t="s">
+        <v>24</v>
+      </c>
+      <c r="D216" s="183" t="s">
+        <v>51</v>
+      </c>
+      <c r="E216" s="183"/>
+      <c r="F216" s="183" t="s">
+        <v>31</v>
+      </c>
+      <c r="G216" s="183"/>
+      <c r="H216" s="183"/>
+      <c r="I216" s="183"/>
+      <c r="J216" s="183"/>
+      <c r="K216" s="183"/>
+      <c r="L216" s="183"/>
+      <c r="M216" s="183"/>
+      <c r="N216" s="183"/>
+      <c r="O216" s="183"/>
+      <c r="P216" s="183"/>
+      <c r="Q216" s="183"/>
+      <c r="R216" s="183"/>
+      <c r="S216" s="183"/>
+      <c r="T216" s="183"/>
+      <c r="U216" s="183"/>
+      <c r="V216" s="152"/>
+      <c r="W216" s="152"/>
+      <c r="X216" s="152"/>
+      <c r="Y216" s="152"/>
+      <c r="Z216" s="152"/>
+      <c r="AA216" s="152"/>
+      <c r="AB216" s="152"/>
+      <c r="AC216" s="152"/>
+      <c r="AD216" s="152"/>
+      <c r="AE216" s="152"/>
+      <c r="AF216" s="152"/>
+      <c r="AG216" s="152"/>
+      <c r="AH216" s="152"/>
+      <c r="AI216" s="152"/>
+    </row>
+    <row r="217" spans="2:35" s="181" customFormat="1">
+      <c r="B217" s="184"/>
+      <c r="C217" s="185"/>
+      <c r="D217" s="185"/>
+      <c r="E217" s="185"/>
+      <c r="F217" s="185"/>
+      <c r="G217" s="185"/>
+      <c r="H217" s="185"/>
+      <c r="I217" s="185"/>
+      <c r="J217" s="185"/>
+      <c r="K217" s="185"/>
+      <c r="L217" s="185"/>
+      <c r="M217" s="185"/>
+      <c r="N217" s="185"/>
+      <c r="O217" s="185"/>
+      <c r="P217" s="185"/>
+      <c r="Q217" s="185"/>
+      <c r="R217" s="185"/>
+      <c r="S217" s="185"/>
+      <c r="T217" s="185"/>
+      <c r="U217" s="185"/>
+      <c r="V217" s="185"/>
+      <c r="W217" s="185"/>
+      <c r="X217" s="185"/>
+      <c r="Y217" s="185"/>
+      <c r="Z217" s="185"/>
+      <c r="AA217" s="185"/>
+      <c r="AB217" s="185"/>
+      <c r="AC217" s="185"/>
+      <c r="AD217" s="185"/>
+      <c r="AE217" s="185"/>
+      <c r="AF217" s="185"/>
+      <c r="AG217" s="185"/>
+      <c r="AH217" s="185"/>
+      <c r="AI217" s="185"/>
+    </row>
+    <row r="218" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B218" s="184"/>
+      <c r="C218" s="186" t="s">
+        <v>186</v>
+      </c>
+      <c r="D218" s="187"/>
+      <c r="E218" s="187"/>
+      <c r="F218" s="187"/>
+      <c r="G218" s="187"/>
+      <c r="H218" s="187"/>
+      <c r="I218" s="187"/>
+      <c r="J218" s="112"/>
+      <c r="K218" s="112"/>
+      <c r="L218" s="112"/>
+      <c r="M218" s="112"/>
+      <c r="N218" s="112"/>
+      <c r="O218" s="112"/>
+      <c r="P218" s="112"/>
+      <c r="Q218" s="112"/>
+      <c r="R218" s="112"/>
+      <c r="S218" s="112"/>
+      <c r="T218" s="112"/>
+      <c r="U218" s="112"/>
+      <c r="V218" s="112"/>
+      <c r="W218" s="112"/>
+      <c r="X218" s="112"/>
+      <c r="Y218" s="112"/>
+      <c r="Z218" s="188"/>
+      <c r="AA218" s="188"/>
+      <c r="AB218" s="188"/>
+      <c r="AC218" s="188"/>
+      <c r="AD218" s="188"/>
+      <c r="AE218" s="188"/>
+      <c r="AF218" s="188"/>
+      <c r="AG218" s="188"/>
+      <c r="AH218" s="188"/>
+      <c r="AI218" s="188"/>
+    </row>
+    <row r="219" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B219" s="184"/>
+      <c r="C219" s="187"/>
+      <c r="D219" s="187"/>
+      <c r="E219" s="187"/>
+      <c r="F219" s="187"/>
+      <c r="G219" s="187"/>
+      <c r="H219" s="187"/>
+      <c r="I219" s="187"/>
+      <c r="J219" s="112"/>
+      <c r="K219" s="112"/>
+      <c r="L219" s="112"/>
+      <c r="M219" s="112"/>
+      <c r="N219" s="112"/>
+      <c r="O219" s="112"/>
+      <c r="P219" s="112"/>
+      <c r="Q219" s="112"/>
+      <c r="R219" s="112"/>
+      <c r="S219" s="112"/>
       <c r="T219" s="112"/>
       <c r="U219" s="112"/>
       <c r="V219" s="112"/>
       <c r="W219" s="112"/>
       <c r="X219" s="112"/>
-      <c r="Y219"/>
-    </row>
-    <row r="220" spans="1:26" customFormat="1" ht="16">
-      <c r="A220" s="101"/>
-      <c r="B220" s="101"/>
-      <c r="C220" s="101"/>
-      <c r="D220" s="101"/>
-      <c r="E220" s="101"/>
-      <c r="F220" s="101"/>
-      <c r="G220" s="101"/>
-      <c r="H220" s="101"/>
-      <c r="I220" s="101"/>
-      <c r="J220" s="101"/>
-      <c r="K220" s="101"/>
-      <c r="L220" s="101"/>
-      <c r="M220" s="101"/>
-      <c r="N220" s="101"/>
-      <c r="O220" s="101"/>
-      <c r="P220" s="101"/>
-      <c r="Q220" s="101"/>
-      <c r="R220" s="101"/>
-      <c r="S220" s="101"/>
+      <c r="Y219" s="112"/>
+      <c r="Z219" s="188"/>
+      <c r="AA219" s="188"/>
+      <c r="AB219" s="188"/>
+      <c r="AC219" s="188"/>
+      <c r="AD219" s="188"/>
+      <c r="AE219" s="188"/>
+      <c r="AF219" s="188"/>
+      <c r="AG219" s="188"/>
+      <c r="AH219" s="188"/>
+      <c r="AI219" s="188"/>
+    </row>
+    <row r="220" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B220" s="184"/>
+      <c r="C220" s="187"/>
+      <c r="D220" s="187"/>
+      <c r="E220" s="187"/>
+      <c r="F220" s="187"/>
+      <c r="G220" s="187"/>
+      <c r="H220" s="187"/>
+      <c r="I220" s="187"/>
+      <c r="J220" s="112"/>
+      <c r="K220" s="112"/>
+      <c r="L220" s="112"/>
+      <c r="M220" s="112"/>
+      <c r="N220" s="112"/>
+      <c r="O220" s="112"/>
+      <c r="P220" s="112"/>
+      <c r="Q220" s="112"/>
+      <c r="R220" s="112"/>
+      <c r="S220" s="112"/>
       <c r="T220" s="112"/>
       <c r="U220" s="112"/>
       <c r="V220" s="112"/>
       <c r="W220" s="112"/>
       <c r="X220" s="112"/>
-      <c r="Z220" s="101"/>
-    </row>
-    <row r="221" spans="1:26" customFormat="1" ht="16">
-      <c r="A221" s="101"/>
-      <c r="B221" s="101"/>
-      <c r="C221" s="101"/>
-      <c r="D221" s="101"/>
-      <c r="E221" s="101"/>
-      <c r="F221" s="101"/>
-      <c r="G221" s="101"/>
-      <c r="H221" s="101"/>
-      <c r="I221" s="101"/>
-      <c r="J221" s="101"/>
-      <c r="K221" s="101"/>
-      <c r="L221" s="101"/>
-      <c r="M221" s="101"/>
-      <c r="N221" s="101"/>
-      <c r="O221" s="101"/>
-      <c r="P221" s="101"/>
-      <c r="Q221" s="101"/>
-      <c r="R221" s="101"/>
-      <c r="S221" s="101"/>
+      <c r="Y220" s="112"/>
+      <c r="Z220" s="188"/>
+      <c r="AA220" s="188"/>
+      <c r="AB220" s="188"/>
+      <c r="AC220" s="188"/>
+      <c r="AD220" s="188"/>
+      <c r="AE220" s="188"/>
+      <c r="AF220" s="188"/>
+      <c r="AG220" s="188"/>
+      <c r="AH220" s="188"/>
+      <c r="AI220" s="188"/>
+    </row>
+    <row r="221" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B221" s="184"/>
+      <c r="C221" s="187"/>
+      <c r="D221" s="192"/>
+      <c r="E221" s="192"/>
+      <c r="F221" s="192"/>
+      <c r="G221" s="192"/>
+      <c r="H221" s="192"/>
+      <c r="I221" s="192"/>
+      <c r="J221" s="143"/>
+      <c r="K221" s="112"/>
+      <c r="L221" s="112"/>
+      <c r="M221" s="112"/>
+      <c r="N221" s="112"/>
+      <c r="O221" s="112"/>
+      <c r="P221" s="112"/>
+      <c r="Q221" s="112"/>
+      <c r="R221" s="112"/>
+      <c r="S221" s="112"/>
       <c r="T221" s="112"/>
       <c r="U221" s="112"/>
       <c r="V221" s="112"/>
       <c r="W221" s="112"/>
       <c r="X221" s="112"/>
-      <c r="Z221" s="101"/>
-    </row>
-    <row r="222" spans="1:26" customFormat="1" ht="16">
-      <c r="A222" s="101"/>
-      <c r="B222" s="101"/>
-      <c r="C222" s="101"/>
-      <c r="D222" s="101"/>
-      <c r="E222" s="101"/>
-      <c r="F222" s="101"/>
-      <c r="G222" s="101"/>
-      <c r="H222" s="101"/>
-      <c r="I222" s="101"/>
-      <c r="J222" s="101"/>
-      <c r="K222" s="101"/>
-      <c r="L222" s="101"/>
-      <c r="M222" s="101"/>
-      <c r="N222" s="101"/>
-      <c r="O222" s="101"/>
-      <c r="P222" s="101"/>
-      <c r="Q222" s="101"/>
-      <c r="R222" s="101"/>
-      <c r="S222" s="101"/>
+      <c r="Y221" s="112"/>
+      <c r="Z221" s="188"/>
+      <c r="AA221" s="188"/>
+      <c r="AB221" s="188"/>
+      <c r="AC221" s="188"/>
+      <c r="AD221" s="188"/>
+      <c r="AE221" s="188"/>
+      <c r="AF221" s="188"/>
+      <c r="AG221" s="188"/>
+      <c r="AH221" s="188"/>
+      <c r="AI221" s="188"/>
+    </row>
+    <row r="222" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B222" s="184"/>
+      <c r="C222" s="187"/>
+      <c r="D222" s="192"/>
+      <c r="E222" s="192"/>
+      <c r="F222" s="192"/>
+      <c r="G222" s="192"/>
+      <c r="H222" s="192"/>
+      <c r="I222" s="192"/>
+      <c r="J222" s="143"/>
+      <c r="K222" s="112"/>
+      <c r="L222" s="112"/>
+      <c r="M222" s="112"/>
+      <c r="N222" s="112"/>
+      <c r="O222" s="112"/>
+      <c r="P222" s="112"/>
+      <c r="Q222" s="112"/>
+      <c r="R222" s="112"/>
+      <c r="S222" s="112"/>
       <c r="T222" s="112"/>
       <c r="U222" s="112"/>
       <c r="V222" s="112"/>
       <c r="W222" s="112"/>
       <c r="X222" s="112"/>
-      <c r="Z222" s="101"/>
-    </row>
-    <row r="223" spans="1:26" customFormat="1" ht="16">
-      <c r="A223" s="101"/>
-      <c r="B223" s="101"/>
-      <c r="C223" s="101"/>
-      <c r="D223" s="101"/>
-      <c r="E223" s="101"/>
-      <c r="F223" s="101"/>
-      <c r="G223" s="101"/>
-      <c r="H223" s="101"/>
-      <c r="I223" s="101"/>
-      <c r="J223" s="101"/>
-      <c r="K223" s="101"/>
-      <c r="L223" s="101"/>
-      <c r="M223" s="101"/>
-      <c r="N223" s="101"/>
-      <c r="O223" s="101"/>
-      <c r="P223" s="101"/>
-      <c r="Q223" s="101"/>
-      <c r="R223" s="101"/>
-      <c r="S223" s="101"/>
+      <c r="Y222" s="112"/>
+      <c r="Z222" s="188"/>
+      <c r="AA222" s="188"/>
+      <c r="AB222" s="188"/>
+      <c r="AC222" s="188"/>
+      <c r="AD222" s="188"/>
+      <c r="AE222" s="188"/>
+      <c r="AF222" s="188"/>
+      <c r="AG222" s="188"/>
+      <c r="AH222" s="188"/>
+      <c r="AI222" s="188"/>
+    </row>
+    <row r="223" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B223" s="184"/>
+      <c r="C223" s="187"/>
+      <c r="D223" s="193"/>
+      <c r="E223" s="193"/>
+      <c r="F223" s="193"/>
+      <c r="G223" s="193"/>
+      <c r="H223" s="193"/>
+      <c r="I223" s="193"/>
+      <c r="J223" s="143"/>
+      <c r="K223" s="112"/>
+      <c r="L223" s="112"/>
+      <c r="M223" s="112"/>
+      <c r="N223" s="112"/>
+      <c r="O223" s="112"/>
+      <c r="P223" s="112"/>
+      <c r="Q223" s="112"/>
+      <c r="R223" s="112"/>
+      <c r="S223" s="112"/>
       <c r="T223" s="112"/>
       <c r="U223" s="112"/>
       <c r="V223" s="112"/>
       <c r="W223" s="112"/>
       <c r="X223" s="112"/>
-      <c r="Z223" s="101"/>
-    </row>
-    <row r="224" spans="1:26" customFormat="1" ht="16">
-      <c r="A224" s="101"/>
-      <c r="B224" s="101"/>
-      <c r="C224" s="101"/>
-      <c r="D224" s="101"/>
-      <c r="E224" s="101"/>
-      <c r="F224" s="101"/>
-      <c r="G224" s="101"/>
-      <c r="H224" s="101"/>
-      <c r="I224" s="101"/>
-      <c r="J224" s="101"/>
-      <c r="K224" s="101"/>
-      <c r="L224" s="101"/>
-      <c r="M224" s="101"/>
-      <c r="N224" s="101"/>
-      <c r="O224" s="101"/>
-      <c r="P224" s="101"/>
-      <c r="Q224" s="101"/>
-      <c r="R224" s="101"/>
-      <c r="S224" s="101"/>
+      <c r="Y223" s="112"/>
+      <c r="Z223" s="188"/>
+      <c r="AA223" s="188"/>
+      <c r="AB223" s="188"/>
+      <c r="AC223" s="188"/>
+      <c r="AD223" s="188"/>
+      <c r="AE223" s="188"/>
+      <c r="AF223" s="188"/>
+      <c r="AG223" s="188"/>
+      <c r="AH223" s="188"/>
+      <c r="AI223" s="188"/>
+    </row>
+    <row r="224" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B224" s="184"/>
+      <c r="C224" s="187"/>
+      <c r="D224" s="193"/>
+      <c r="E224" s="193"/>
+      <c r="F224" s="193"/>
+      <c r="G224" s="193"/>
+      <c r="H224" s="193"/>
+      <c r="I224" s="193"/>
+      <c r="J224" s="143"/>
+      <c r="K224" s="112"/>
+      <c r="L224" s="112"/>
+      <c r="M224" s="112"/>
+      <c r="N224" s="112"/>
+      <c r="O224" s="112"/>
+      <c r="P224" s="112"/>
+      <c r="Q224" s="112"/>
+      <c r="R224" s="112"/>
+      <c r="S224" s="112"/>
       <c r="T224" s="112"/>
       <c r="U224" s="112"/>
       <c r="V224" s="112"/>
       <c r="W224" s="112"/>
       <c r="X224" s="112"/>
-      <c r="Z224" s="101"/>
-    </row>
-    <row r="225" spans="1:26" customFormat="1" ht="16">
-      <c r="A225" s="101"/>
-      <c r="B225" s="101"/>
-      <c r="C225" s="101"/>
-      <c r="D225" s="101"/>
-      <c r="E225" s="101"/>
-      <c r="F225" s="101"/>
-      <c r="G225" s="101"/>
-      <c r="H225" s="101"/>
-      <c r="I225" s="101"/>
-      <c r="J225" s="101"/>
-      <c r="K225" s="101"/>
-      <c r="L225" s="101"/>
-      <c r="M225" s="101"/>
-      <c r="N225" s="101"/>
-      <c r="O225" s="101"/>
-      <c r="P225" s="101"/>
-      <c r="Q225" s="101"/>
-      <c r="R225" s="101"/>
-      <c r="S225" s="101"/>
+      <c r="Y224" s="112"/>
+      <c r="Z224" s="188"/>
+      <c r="AA224" s="188"/>
+      <c r="AB224" s="188"/>
+      <c r="AC224" s="188"/>
+      <c r="AD224" s="188"/>
+      <c r="AE224" s="188"/>
+      <c r="AF224" s="188"/>
+      <c r="AG224" s="188"/>
+      <c r="AH224" s="188"/>
+      <c r="AI224" s="188"/>
+    </row>
+    <row r="225" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B225" s="184"/>
+      <c r="C225" s="187"/>
+      <c r="D225" s="193"/>
+      <c r="E225" s="193"/>
+      <c r="F225" s="193"/>
+      <c r="G225" s="193"/>
+      <c r="H225" s="193"/>
+      <c r="I225" s="193"/>
+      <c r="J225" s="143"/>
+      <c r="K225" s="112"/>
+      <c r="L225" s="112"/>
+      <c r="M225" s="112"/>
+      <c r="N225" s="112"/>
+      <c r="O225" s="112"/>
+      <c r="P225" s="112"/>
+      <c r="Q225" s="112"/>
+      <c r="R225" s="112"/>
+      <c r="S225" s="112"/>
       <c r="T225" s="112"/>
       <c r="U225" s="112"/>
       <c r="V225" s="112"/>
       <c r="W225" s="112"/>
       <c r="X225" s="112"/>
-      <c r="Z225" s="101"/>
-    </row>
-    <row r="226" spans="1:26" customFormat="1" ht="16">
-      <c r="A226" s="101"/>
-      <c r="B226" s="101"/>
-      <c r="C226" s="101"/>
-      <c r="D226" s="101"/>
-      <c r="E226" s="101"/>
-      <c r="F226" s="101"/>
-      <c r="G226" s="101"/>
-      <c r="H226" s="101"/>
-      <c r="I226" s="101"/>
-      <c r="J226" s="101"/>
-      <c r="K226" s="101"/>
-      <c r="L226" s="101"/>
-      <c r="M226" s="101"/>
-      <c r="N226" s="101"/>
-      <c r="O226" s="101"/>
-      <c r="P226" s="101"/>
-      <c r="Q226" s="101"/>
-      <c r="R226" s="101"/>
-      <c r="S226" s="101"/>
+      <c r="Y225" s="112"/>
+      <c r="Z225" s="188"/>
+      <c r="AA225" s="188"/>
+      <c r="AB225" s="188"/>
+      <c r="AC225" s="188"/>
+      <c r="AD225" s="188"/>
+      <c r="AE225" s="188"/>
+      <c r="AF225" s="188"/>
+      <c r="AG225" s="188"/>
+      <c r="AH225" s="188"/>
+      <c r="AI225" s="188"/>
+    </row>
+    <row r="226" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B226" s="184"/>
+      <c r="C226" s="112"/>
+      <c r="D226" s="143"/>
+      <c r="E226" s="143"/>
+      <c r="F226" s="143"/>
+      <c r="G226" s="143"/>
+      <c r="H226" s="143"/>
+      <c r="I226" s="143"/>
+      <c r="J226" s="143"/>
+      <c r="K226" s="112"/>
+      <c r="L226" s="112"/>
+      <c r="M226" s="112"/>
+      <c r="N226" s="112"/>
+      <c r="O226" s="112"/>
+      <c r="P226" s="112"/>
+      <c r="Q226" s="112"/>
+      <c r="R226" s="112"/>
+      <c r="S226" s="112"/>
       <c r="T226" s="112"/>
       <c r="U226" s="112"/>
       <c r="V226" s="112"/>
       <c r="W226" s="112"/>
       <c r="X226" s="112"/>
-      <c r="Z226" s="101"/>
-    </row>
-    <row r="227" spans="1:26" customFormat="1" ht="16">
-      <c r="A227" s="101"/>
-      <c r="B227" s="101"/>
-      <c r="C227" s="101"/>
-      <c r="D227" s="101"/>
-      <c r="E227" s="101"/>
-      <c r="F227" s="101"/>
-      <c r="G227" s="101"/>
-      <c r="H227" s="101"/>
-      <c r="I227" s="101"/>
-      <c r="J227" s="101"/>
-      <c r="K227" s="101"/>
-      <c r="L227" s="101"/>
-      <c r="M227" s="101"/>
-      <c r="N227" s="101"/>
-      <c r="O227" s="101"/>
-      <c r="P227" s="101"/>
-      <c r="Q227" s="101"/>
-      <c r="R227" s="101"/>
-      <c r="S227" s="101"/>
+      <c r="Y226" s="112"/>
+      <c r="Z226" s="188"/>
+      <c r="AA226" s="188"/>
+      <c r="AB226" s="188"/>
+      <c r="AC226" s="188"/>
+      <c r="AD226" s="188"/>
+      <c r="AE226" s="188"/>
+      <c r="AF226" s="188"/>
+      <c r="AG226" s="188"/>
+      <c r="AH226" s="188"/>
+      <c r="AI226" s="188"/>
+    </row>
+    <row r="227" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B227" s="184"/>
+      <c r="C227" s="112"/>
+      <c r="D227" s="143"/>
+      <c r="E227" s="143"/>
+      <c r="F227" s="143"/>
+      <c r="G227" s="143"/>
+      <c r="H227" s="143"/>
+      <c r="I227" s="143"/>
+      <c r="J227" s="143"/>
+      <c r="K227" s="112"/>
+      <c r="L227" s="112"/>
+      <c r="M227" s="112"/>
+      <c r="N227" s="112"/>
+      <c r="O227" s="112"/>
+      <c r="P227" s="112"/>
+      <c r="Q227" s="112"/>
+      <c r="R227" s="112"/>
+      <c r="S227" s="112"/>
       <c r="T227" s="112"/>
       <c r="U227" s="112"/>
       <c r="V227" s="112"/>
       <c r="W227" s="112"/>
       <c r="X227" s="112"/>
-      <c r="Z227" s="101"/>
-    </row>
-    <row r="228" spans="1:26" customFormat="1" ht="16">
-      <c r="A228" s="101"/>
-      <c r="B228" s="101"/>
-      <c r="C228" s="101"/>
-      <c r="D228" s="101"/>
-      <c r="E228" s="101"/>
-      <c r="F228" s="101"/>
-      <c r="G228" s="101"/>
-      <c r="H228" s="101"/>
-      <c r="I228" s="101"/>
-      <c r="J228" s="101"/>
-      <c r="K228" s="101"/>
-      <c r="L228" s="101"/>
-      <c r="M228" s="101"/>
-      <c r="N228" s="101"/>
-      <c r="O228" s="101"/>
-      <c r="P228" s="101"/>
-      <c r="Q228" s="101"/>
-      <c r="R228" s="101"/>
-      <c r="S228" s="101"/>
+      <c r="Y227" s="112"/>
+      <c r="Z227" s="188"/>
+      <c r="AA227" s="188"/>
+      <c r="AB227" s="188"/>
+      <c r="AC227" s="188"/>
+      <c r="AD227" s="188"/>
+      <c r="AE227" s="188"/>
+      <c r="AF227" s="188"/>
+      <c r="AG227" s="188"/>
+      <c r="AH227" s="188"/>
+      <c r="AI227" s="188"/>
+    </row>
+    <row r="228" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B228" s="184"/>
+      <c r="C228" s="112"/>
+      <c r="D228" s="143"/>
+      <c r="E228" s="143"/>
+      <c r="F228" s="143"/>
+      <c r="G228" s="143"/>
+      <c r="H228" s="143"/>
+      <c r="I228" s="143"/>
+      <c r="J228" s="143"/>
+      <c r="K228" s="112"/>
+      <c r="L228" s="112"/>
+      <c r="M228" s="112"/>
+      <c r="N228" s="112"/>
+      <c r="O228" s="112"/>
+      <c r="P228" s="112"/>
+      <c r="Q228" s="112"/>
+      <c r="R228" s="112"/>
+      <c r="S228" s="112"/>
       <c r="T228" s="112"/>
       <c r="U228" s="112"/>
       <c r="V228" s="112"/>
       <c r="W228" s="112"/>
       <c r="X228" s="112"/>
-      <c r="Z228" s="101"/>
-    </row>
-    <row r="229" spans="1:26" customFormat="1" ht="16">
-      <c r="A229" s="101"/>
-      <c r="B229" s="101"/>
-      <c r="C229" s="101"/>
-      <c r="D229" s="101"/>
-      <c r="E229" s="101"/>
-      <c r="F229" s="101"/>
-      <c r="G229" s="101"/>
-      <c r="H229" s="101"/>
-      <c r="I229" s="101"/>
-      <c r="J229" s="101"/>
-      <c r="K229" s="101"/>
-      <c r="L229" s="101"/>
-      <c r="M229" s="101"/>
-      <c r="N229" s="101"/>
-      <c r="O229" s="101"/>
-      <c r="P229" s="101"/>
-      <c r="Q229" s="101"/>
-      <c r="R229" s="101"/>
-      <c r="S229" s="101"/>
+      <c r="Y228" s="112"/>
+      <c r="Z228" s="188"/>
+      <c r="AA228" s="188"/>
+      <c r="AB228" s="188"/>
+      <c r="AC228" s="188"/>
+      <c r="AD228" s="188"/>
+      <c r="AE228" s="188"/>
+      <c r="AF228" s="188"/>
+      <c r="AG228" s="188"/>
+      <c r="AH228" s="188"/>
+      <c r="AI228" s="188"/>
+    </row>
+    <row r="229" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B229" s="184"/>
+      <c r="C229" s="112"/>
+      <c r="D229" s="143"/>
+      <c r="E229" s="143"/>
+      <c r="F229" s="143"/>
+      <c r="G229" s="143"/>
+      <c r="H229" s="143"/>
+      <c r="I229" s="143"/>
+      <c r="J229" s="143"/>
+      <c r="K229" s="112"/>
+      <c r="L229" s="112"/>
+      <c r="M229" s="112"/>
+      <c r="N229" s="112"/>
+      <c r="O229" s="112"/>
+      <c r="P229" s="112"/>
+      <c r="Q229" s="112"/>
+      <c r="R229" s="112"/>
+      <c r="S229" s="112"/>
       <c r="T229" s="112"/>
       <c r="U229" s="112"/>
       <c r="V229" s="112"/>
       <c r="W229" s="112"/>
       <c r="X229" s="112"/>
-      <c r="Z229" s="101"/>
-    </row>
-    <row r="230" spans="1:26" customFormat="1" ht="16">
-      <c r="A230" s="101"/>
-      <c r="B230" s="101"/>
-      <c r="C230" s="101"/>
-      <c r="D230" s="101"/>
-      <c r="E230" s="101"/>
-      <c r="F230" s="101"/>
-      <c r="G230" s="101"/>
-      <c r="H230" s="101"/>
-      <c r="I230" s="101"/>
-      <c r="J230" s="101"/>
-      <c r="K230" s="101"/>
-      <c r="L230" s="101"/>
-      <c r="M230" s="101"/>
-      <c r="N230" s="101"/>
-      <c r="O230" s="101"/>
-      <c r="P230" s="101"/>
-      <c r="Q230" s="101"/>
-      <c r="R230" s="101"/>
-      <c r="S230" s="101"/>
+      <c r="Y229" s="112"/>
+      <c r="Z229" s="188"/>
+      <c r="AA229" s="188"/>
+      <c r="AB229" s="188"/>
+      <c r="AC229" s="188"/>
+      <c r="AD229" s="188"/>
+      <c r="AE229" s="188"/>
+      <c r="AF229" s="188"/>
+      <c r="AG229" s="188"/>
+      <c r="AH229" s="188"/>
+      <c r="AI229" s="188"/>
+    </row>
+    <row r="230" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B230" s="184"/>
+      <c r="C230" s="112"/>
+      <c r="D230" s="143"/>
+      <c r="E230" s="143"/>
+      <c r="F230" s="143"/>
+      <c r="G230" s="143"/>
+      <c r="H230" s="143"/>
+      <c r="I230" s="143"/>
+      <c r="J230" s="143"/>
+      <c r="K230" s="112"/>
+      <c r="L230" s="112"/>
+      <c r="M230" s="112"/>
+      <c r="N230" s="112"/>
+      <c r="O230" s="112"/>
+      <c r="P230" s="112"/>
+      <c r="Q230" s="112"/>
+      <c r="R230" s="112"/>
+      <c r="S230" s="112"/>
       <c r="T230" s="112"/>
       <c r="U230" s="112"/>
       <c r="V230" s="112"/>
       <c r="W230" s="112"/>
       <c r="X230" s="112"/>
-      <c r="Z230" s="101"/>
-    </row>
-    <row r="231" spans="1:26" customFormat="1" ht="16">
-      <c r="A231" s="101"/>
-      <c r="B231" s="101"/>
-      <c r="C231" s="101"/>
-      <c r="D231" s="101"/>
-      <c r="E231" s="101"/>
-      <c r="F231" s="101"/>
-      <c r="G231" s="101"/>
-      <c r="H231" s="101"/>
-      <c r="I231" s="101"/>
-      <c r="J231" s="101"/>
-      <c r="K231" s="101"/>
-      <c r="L231" s="101"/>
-      <c r="M231" s="101"/>
-      <c r="N231" s="101"/>
-      <c r="O231" s="101"/>
-      <c r="P231" s="101"/>
-      <c r="Q231" s="101"/>
-      <c r="R231" s="101"/>
-      <c r="S231" s="101"/>
+      <c r="Y230" s="112"/>
+      <c r="Z230" s="188"/>
+      <c r="AA230" s="188"/>
+      <c r="AB230" s="188"/>
+      <c r="AC230" s="188"/>
+      <c r="AD230" s="188"/>
+      <c r="AE230" s="188"/>
+      <c r="AF230" s="188"/>
+      <c r="AG230" s="188"/>
+      <c r="AH230" s="188"/>
+      <c r="AI230" s="188"/>
+    </row>
+    <row r="231" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B231" s="184"/>
+      <c r="C231" s="112"/>
+      <c r="D231" s="143"/>
+      <c r="E231" s="143"/>
+      <c r="F231" s="143"/>
+      <c r="G231" s="143"/>
+      <c r="H231" s="143"/>
+      <c r="I231" s="143"/>
+      <c r="J231" s="143"/>
+      <c r="K231" s="112"/>
+      <c r="L231" s="112"/>
+      <c r="M231" s="112"/>
+      <c r="N231" s="112"/>
+      <c r="O231" s="112"/>
+      <c r="P231" s="112"/>
+      <c r="Q231" s="112"/>
+      <c r="R231" s="112"/>
+      <c r="S231" s="112"/>
       <c r="T231" s="112"/>
       <c r="U231" s="112"/>
       <c r="V231" s="112"/>
       <c r="W231" s="112"/>
       <c r="X231" s="112"/>
-      <c r="Z231" s="101"/>
-    </row>
-    <row r="232" spans="1:26" customFormat="1" ht="16">
-      <c r="A232" s="101"/>
-      <c r="B232" s="101"/>
-      <c r="C232" s="101"/>
-      <c r="D232" s="101"/>
-      <c r="E232" s="101"/>
-      <c r="F232" s="101"/>
-      <c r="G232" s="101"/>
-      <c r="H232" s="101"/>
-      <c r="I232" s="101"/>
-      <c r="J232" s="101"/>
-      <c r="K232" s="101"/>
-      <c r="L232" s="101"/>
-      <c r="M232" s="101"/>
-      <c r="N232" s="101"/>
-      <c r="O232" s="101"/>
-      <c r="P232" s="101"/>
-      <c r="Q232" s="101"/>
-      <c r="R232" s="101"/>
-      <c r="S232" s="101"/>
+      <c r="Y231" s="112"/>
+      <c r="Z231" s="188"/>
+      <c r="AA231" s="188"/>
+      <c r="AB231" s="188"/>
+      <c r="AC231" s="188"/>
+      <c r="AD231" s="188"/>
+      <c r="AE231" s="188"/>
+      <c r="AF231" s="188"/>
+      <c r="AG231" s="188"/>
+      <c r="AH231" s="188"/>
+      <c r="AI231" s="188"/>
+    </row>
+    <row r="232" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B232" s="184"/>
+      <c r="C232" s="112"/>
+      <c r="D232" s="143"/>
+      <c r="E232" s="143"/>
+      <c r="F232" s="143"/>
+      <c r="G232" s="143"/>
+      <c r="H232" s="143"/>
+      <c r="I232" s="143"/>
+      <c r="J232" s="143"/>
+      <c r="K232" s="112"/>
+      <c r="L232" s="112"/>
+      <c r="M232" s="112"/>
+      <c r="N232" s="112"/>
+      <c r="O232" s="112"/>
+      <c r="P232" s="112"/>
+      <c r="Q232" s="112"/>
+      <c r="R232" s="112"/>
+      <c r="S232" s="112"/>
       <c r="T232" s="112"/>
       <c r="U232" s="112"/>
       <c r="V232" s="112"/>
       <c r="W232" s="112"/>
       <c r="X232" s="112"/>
-      <c r="Z232" s="101"/>
-    </row>
-    <row r="233" spans="1:26" customFormat="1" ht="16">
-      <c r="A233" s="101"/>
-      <c r="B233" s="101"/>
-      <c r="C233" s="101"/>
-      <c r="D233" s="101"/>
-      <c r="E233" s="101"/>
-      <c r="F233" s="101"/>
-      <c r="G233" s="101"/>
-      <c r="H233" s="101"/>
-      <c r="I233" s="101"/>
-      <c r="J233" s="101"/>
-      <c r="K233" s="101"/>
-      <c r="L233" s="101"/>
-      <c r="M233" s="101"/>
-      <c r="N233" s="101"/>
-      <c r="O233" s="101"/>
-      <c r="P233" s="101"/>
-      <c r="Q233" s="101"/>
-      <c r="R233" s="101"/>
-      <c r="S233" s="101"/>
+      <c r="Y232" s="112"/>
+      <c r="Z232" s="188"/>
+      <c r="AA232" s="188"/>
+      <c r="AB232" s="188"/>
+      <c r="AC232" s="188"/>
+      <c r="AD232" s="188"/>
+      <c r="AE232" s="188"/>
+      <c r="AF232" s="188"/>
+      <c r="AG232" s="188"/>
+      <c r="AH232" s="188"/>
+      <c r="AI232" s="188"/>
+    </row>
+    <row r="233" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B233" s="184"/>
+      <c r="C233" s="112"/>
+      <c r="D233" s="143"/>
+      <c r="E233" s="143"/>
+      <c r="F233" s="143"/>
+      <c r="G233" s="143"/>
+      <c r="H233" s="143"/>
+      <c r="I233" s="143"/>
+      <c r="J233" s="143"/>
+      <c r="K233" s="112"/>
+      <c r="L233" s="112"/>
+      <c r="M233" s="112"/>
+      <c r="N233" s="112"/>
+      <c r="O233" s="112"/>
+      <c r="P233" s="112"/>
+      <c r="Q233" s="112"/>
+      <c r="R233" s="112"/>
+      <c r="S233" s="112"/>
       <c r="T233" s="112"/>
       <c r="U233" s="112"/>
       <c r="V233" s="112"/>
       <c r="W233" s="112"/>
       <c r="X233" s="112"/>
-      <c r="Z233" s="101"/>
-    </row>
-    <row r="234" spans="1:26" customFormat="1" ht="16">
-      <c r="A234" s="101"/>
-      <c r="B234" s="101"/>
-      <c r="C234" s="101"/>
-      <c r="D234" s="101"/>
-      <c r="E234" s="101"/>
-      <c r="F234" s="101"/>
-      <c r="G234" s="101"/>
-      <c r="H234" s="101"/>
-      <c r="I234" s="101"/>
-      <c r="J234" s="101"/>
-      <c r="K234" s="101"/>
-      <c r="L234" s="101"/>
-      <c r="M234" s="101"/>
-      <c r="N234" s="101"/>
-      <c r="O234" s="101"/>
-      <c r="P234" s="101"/>
-      <c r="Q234" s="101"/>
-      <c r="R234" s="101"/>
-      <c r="S234" s="101"/>
+      <c r="Y233" s="112"/>
+      <c r="Z233" s="188"/>
+      <c r="AA233" s="188"/>
+      <c r="AB233" s="188"/>
+      <c r="AC233" s="188"/>
+      <c r="AD233" s="188"/>
+      <c r="AE233" s="188"/>
+      <c r="AF233" s="188"/>
+      <c r="AG233" s="188"/>
+      <c r="AH233" s="188"/>
+      <c r="AI233" s="188"/>
+    </row>
+    <row r="234" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B234" s="184"/>
+      <c r="C234" s="112"/>
+      <c r="D234" s="112"/>
+      <c r="E234" s="112"/>
+      <c r="F234" s="112"/>
+      <c r="G234" s="112"/>
+      <c r="H234" s="112"/>
+      <c r="I234" s="112"/>
+      <c r="J234" s="112"/>
+      <c r="K234" s="112"/>
+      <c r="L234" s="112"/>
+      <c r="M234" s="112"/>
+      <c r="N234" s="112"/>
+      <c r="O234" s="112"/>
+      <c r="P234" s="112"/>
+      <c r="Q234" s="112"/>
+      <c r="R234" s="112"/>
+      <c r="S234" s="112"/>
       <c r="T234" s="112"/>
       <c r="U234" s="112"/>
       <c r="V234" s="112"/>
       <c r="W234" s="112"/>
       <c r="X234" s="112"/>
-      <c r="Z234" s="101"/>
-    </row>
-    <row r="235" spans="1:26" customFormat="1" ht="16">
-      <c r="A235" s="101"/>
-      <c r="B235" s="101"/>
-      <c r="C235" s="101"/>
-      <c r="D235" s="101"/>
-      <c r="E235" s="101"/>
-      <c r="F235" s="101"/>
-      <c r="G235" s="101"/>
-      <c r="H235" s="101"/>
-      <c r="I235" s="101"/>
-      <c r="J235" s="101"/>
-      <c r="K235" s="101"/>
-      <c r="L235" s="101"/>
-      <c r="M235" s="101"/>
-      <c r="N235" s="101"/>
-      <c r="O235" s="101"/>
-      <c r="P235" s="101"/>
-      <c r="Q235" s="101"/>
-      <c r="R235" s="101"/>
-      <c r="S235" s="101"/>
+      <c r="Y234" s="112"/>
+      <c r="Z234" s="188"/>
+      <c r="AA234" s="188"/>
+      <c r="AB234" s="188"/>
+      <c r="AC234" s="188"/>
+      <c r="AD234" s="188"/>
+      <c r="AE234" s="188"/>
+      <c r="AF234" s="188"/>
+      <c r="AG234" s="188"/>
+      <c r="AH234" s="188"/>
+      <c r="AI234" s="188"/>
+    </row>
+    <row r="235" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B235" s="184"/>
+      <c r="C235" s="112"/>
+      <c r="D235" s="112"/>
+      <c r="E235" s="112"/>
+      <c r="F235" s="112"/>
+      <c r="G235" s="112"/>
+      <c r="H235" s="112"/>
+      <c r="I235" s="112"/>
+      <c r="J235" s="112"/>
+      <c r="K235" s="112"/>
+      <c r="L235" s="112"/>
+      <c r="M235" s="112"/>
+      <c r="N235" s="112"/>
+      <c r="O235" s="112"/>
+      <c r="P235" s="112"/>
+      <c r="Q235" s="112"/>
+      <c r="R235" s="112"/>
+      <c r="S235" s="112"/>
       <c r="T235" s="112"/>
       <c r="U235" s="112"/>
       <c r="V235" s="112"/>
       <c r="W235" s="112"/>
       <c r="X235" s="112"/>
-      <c r="Z235" s="101"/>
-    </row>
-    <row r="236" spans="1:26" customFormat="1" ht="16">
-      <c r="A236" s="101"/>
-      <c r="B236" s="101"/>
-      <c r="C236" s="101"/>
-      <c r="D236" s="101"/>
-      <c r="E236" s="101"/>
-      <c r="F236" s="101"/>
-      <c r="G236" s="101"/>
-      <c r="H236" s="101"/>
-      <c r="I236" s="101"/>
-      <c r="J236" s="101"/>
-      <c r="K236" s="101"/>
-      <c r="L236" s="101"/>
-      <c r="M236" s="101"/>
-      <c r="N236" s="101"/>
-      <c r="O236" s="101"/>
-      <c r="P236" s="101"/>
-      <c r="Q236" s="101"/>
-      <c r="R236" s="101"/>
-      <c r="S236" s="101"/>
+      <c r="Y235" s="112"/>
+      <c r="Z235" s="188"/>
+      <c r="AA235" s="188"/>
+      <c r="AB235" s="188"/>
+      <c r="AC235" s="188"/>
+      <c r="AD235" s="188"/>
+      <c r="AE235" s="188"/>
+      <c r="AF235" s="188"/>
+      <c r="AG235" s="188"/>
+      <c r="AH235" s="188"/>
+      <c r="AI235" s="188"/>
+    </row>
+    <row r="236" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B236" s="184"/>
+      <c r="C236" s="112"/>
+      <c r="D236" s="112"/>
+      <c r="E236" s="112"/>
+      <c r="F236" s="112"/>
+      <c r="G236" s="112"/>
+      <c r="H236" s="112"/>
+      <c r="I236" s="112"/>
+      <c r="J236" s="112"/>
+      <c r="K236" s="112"/>
+      <c r="L236" s="112"/>
+      <c r="M236" s="112"/>
+      <c r="N236" s="112"/>
+      <c r="O236" s="112"/>
+      <c r="P236" s="112"/>
+      <c r="Q236" s="112"/>
+      <c r="R236" s="112"/>
+      <c r="S236" s="112"/>
       <c r="T236" s="112"/>
       <c r="U236" s="112"/>
       <c r="V236" s="112"/>
       <c r="W236" s="112"/>
       <c r="X236" s="112"/>
-      <c r="Z236" s="101"/>
-    </row>
-    <row r="237" spans="1:26" customFormat="1" ht="16">
-      <c r="A237" s="101"/>
-      <c r="B237" s="101"/>
-      <c r="C237" s="101"/>
-      <c r="D237" s="101"/>
-      <c r="E237" s="101"/>
-      <c r="F237" s="101"/>
-      <c r="G237" s="101"/>
-      <c r="H237" s="101"/>
-      <c r="I237" s="101"/>
-      <c r="J237" s="101"/>
-      <c r="K237" s="101"/>
-      <c r="L237" s="101"/>
-      <c r="M237" s="101"/>
-      <c r="N237" s="101"/>
-      <c r="O237" s="101"/>
-      <c r="P237" s="101"/>
-      <c r="Q237" s="101"/>
-      <c r="R237" s="101"/>
-      <c r="S237" s="101"/>
+      <c r="Y236" s="112"/>
+      <c r="Z236" s="188"/>
+      <c r="AA236" s="188"/>
+      <c r="AB236" s="188"/>
+      <c r="AC236" s="188"/>
+      <c r="AD236" s="188"/>
+      <c r="AE236" s="188"/>
+      <c r="AF236" s="188"/>
+      <c r="AG236" s="188"/>
+      <c r="AH236" s="188"/>
+      <c r="AI236" s="188"/>
+    </row>
+    <row r="237" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B237" s="184"/>
+      <c r="C237" s="112"/>
+      <c r="D237" s="112"/>
+      <c r="E237" s="112"/>
+      <c r="F237" s="112"/>
+      <c r="G237" s="112"/>
+      <c r="H237" s="112"/>
+      <c r="I237" s="112"/>
+      <c r="J237" s="112"/>
+      <c r="K237" s="112"/>
+      <c r="L237" s="112"/>
+      <c r="M237" s="112"/>
+      <c r="N237" s="112"/>
+      <c r="O237" s="112"/>
+      <c r="P237" s="112"/>
+      <c r="Q237" s="112"/>
+      <c r="R237" s="112"/>
+      <c r="S237" s="112"/>
       <c r="T237" s="112"/>
       <c r="U237" s="112"/>
       <c r="V237" s="112"/>
       <c r="W237" s="112"/>
       <c r="X237" s="112"/>
-      <c r="Z237" s="101"/>
-    </row>
-    <row r="238" spans="1:26" customFormat="1" ht="16">
-      <c r="A238" s="101"/>
-      <c r="B238" s="101"/>
-      <c r="C238" s="101"/>
-      <c r="D238" s="101"/>
-      <c r="E238" s="101"/>
-      <c r="F238" s="101"/>
-      <c r="G238" s="101"/>
-      <c r="H238" s="101"/>
-      <c r="I238" s="101"/>
-      <c r="J238" s="101"/>
-      <c r="K238" s="101"/>
-      <c r="L238" s="101"/>
-      <c r="M238" s="101"/>
-      <c r="N238" s="101"/>
-      <c r="O238" s="101"/>
-      <c r="P238" s="101"/>
-      <c r="Q238" s="101"/>
-      <c r="R238" s="101"/>
-      <c r="S238" s="101"/>
+      <c r="Y237" s="112"/>
+      <c r="Z237" s="188"/>
+      <c r="AA237" s="188"/>
+      <c r="AB237" s="188"/>
+      <c r="AC237" s="188"/>
+      <c r="AD237" s="188"/>
+      <c r="AE237" s="188"/>
+      <c r="AF237" s="188"/>
+      <c r="AG237" s="188"/>
+      <c r="AH237" s="188"/>
+      <c r="AI237" s="188"/>
+    </row>
+    <row r="238" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B238" s="184"/>
+      <c r="C238" s="112"/>
+      <c r="D238" s="112"/>
+      <c r="E238" s="112"/>
+      <c r="F238" s="112"/>
+      <c r="G238" s="112"/>
+      <c r="H238" s="112"/>
+      <c r="I238" s="112"/>
+      <c r="J238" s="112"/>
+      <c r="K238" s="112"/>
+      <c r="L238" s="112"/>
+      <c r="M238" s="112"/>
+      <c r="N238" s="112"/>
+      <c r="O238" s="112"/>
+      <c r="P238" s="112"/>
+      <c r="Q238" s="112"/>
+      <c r="R238" s="112"/>
+      <c r="S238" s="112"/>
       <c r="T238" s="112"/>
       <c r="U238" s="112"/>
       <c r="V238" s="112"/>
       <c r="W238" s="112"/>
       <c r="X238" s="112"/>
-      <c r="Z238" s="101"/>
-    </row>
-    <row r="239" spans="1:26" customFormat="1" ht="16">
-      <c r="A239" s="101"/>
-      <c r="B239" s="101"/>
-      <c r="C239" s="101"/>
-      <c r="D239" s="101"/>
-      <c r="E239" s="101"/>
-      <c r="F239" s="101"/>
-      <c r="G239" s="101"/>
-      <c r="H239" s="101"/>
-      <c r="I239" s="101"/>
-      <c r="J239" s="101"/>
-      <c r="K239" s="101"/>
-      <c r="L239" s="101"/>
-      <c r="M239" s="101"/>
-      <c r="N239" s="101"/>
-      <c r="O239" s="101"/>
-      <c r="P239" s="101"/>
-      <c r="Q239" s="101"/>
-      <c r="R239" s="101"/>
-      <c r="S239" s="101"/>
+      <c r="Y238" s="112"/>
+      <c r="Z238" s="188"/>
+      <c r="AA238" s="188"/>
+      <c r="AB238" s="188"/>
+      <c r="AC238" s="188"/>
+      <c r="AD238" s="188"/>
+      <c r="AE238" s="188"/>
+      <c r="AF238" s="188"/>
+      <c r="AG238" s="188"/>
+      <c r="AH238" s="188"/>
+      <c r="AI238" s="188"/>
+    </row>
+    <row r="239" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B239" s="184"/>
+      <c r="C239" s="112"/>
+      <c r="D239" s="112"/>
+      <c r="E239" s="112"/>
+      <c r="F239" s="112"/>
+      <c r="G239" s="112"/>
+      <c r="H239" s="112"/>
+      <c r="I239" s="112"/>
+      <c r="J239" s="112"/>
+      <c r="K239" s="112"/>
+      <c r="L239" s="112"/>
+      <c r="M239" s="112"/>
+      <c r="N239" s="112"/>
+      <c r="O239" s="112"/>
+      <c r="P239" s="112"/>
+      <c r="Q239" s="112"/>
+      <c r="R239" s="112"/>
+      <c r="S239" s="112"/>
       <c r="T239" s="112"/>
       <c r="U239" s="112"/>
       <c r="V239" s="112"/>
       <c r="W239" s="112"/>
       <c r="X239" s="112"/>
-      <c r="Z239" s="101"/>
-    </row>
-    <row r="240" spans="1:26" customFormat="1" ht="16">
-      <c r="A240" s="101"/>
-      <c r="B240" s="101"/>
-      <c r="C240" s="101"/>
-      <c r="D240" s="101"/>
-      <c r="E240" s="101"/>
-      <c r="F240" s="101"/>
-      <c r="G240" s="101"/>
-      <c r="H240" s="101"/>
-      <c r="I240" s="101"/>
-      <c r="J240" s="101"/>
-      <c r="K240" s="101"/>
-      <c r="L240" s="101"/>
-      <c r="M240" s="101"/>
-      <c r="N240" s="101"/>
-      <c r="O240" s="101"/>
-      <c r="P240" s="101"/>
-      <c r="Q240" s="101"/>
-      <c r="R240" s="101"/>
-      <c r="S240" s="101"/>
+      <c r="Y239" s="112"/>
+      <c r="Z239" s="188"/>
+      <c r="AA239" s="188"/>
+      <c r="AB239" s="188"/>
+      <c r="AC239" s="188"/>
+      <c r="AD239" s="188"/>
+      <c r="AE239" s="188"/>
+      <c r="AF239" s="188"/>
+      <c r="AG239" s="188"/>
+      <c r="AH239" s="188"/>
+      <c r="AI239" s="188"/>
+    </row>
+    <row r="240" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B240" s="184"/>
+      <c r="C240" s="112"/>
+      <c r="D240" s="112"/>
+      <c r="E240" s="112"/>
+      <c r="F240" s="112"/>
+      <c r="G240" s="112"/>
+      <c r="H240" s="112"/>
+      <c r="I240" s="112"/>
+      <c r="J240" s="112"/>
+      <c r="K240" s="112"/>
+      <c r="L240" s="112"/>
+      <c r="M240" s="112"/>
+      <c r="N240" s="112"/>
+      <c r="O240" s="112"/>
+      <c r="P240" s="112"/>
+      <c r="Q240" s="112"/>
+      <c r="R240" s="112"/>
+      <c r="S240" s="112"/>
       <c r="T240" s="112"/>
       <c r="U240" s="112"/>
       <c r="V240" s="112"/>
       <c r="W240" s="112"/>
       <c r="X240" s="112"/>
-      <c r="Z240" s="101"/>
-    </row>
-    <row r="241" spans="1:26" customFormat="1" ht="16">
-      <c r="A241" s="101"/>
-      <c r="B241" s="101"/>
-      <c r="C241" s="101"/>
-      <c r="D241" s="101"/>
-      <c r="E241" s="101"/>
-      <c r="F241" s="101"/>
-      <c r="G241" s="101"/>
-      <c r="H241" s="101"/>
-      <c r="I241" s="101"/>
-      <c r="J241" s="101"/>
-      <c r="K241" s="101"/>
-      <c r="L241" s="101"/>
-      <c r="M241" s="101"/>
-      <c r="N241" s="101"/>
-      <c r="O241" s="101"/>
-      <c r="P241" s="101"/>
-      <c r="Q241" s="101"/>
-      <c r="R241" s="101"/>
-      <c r="S241" s="101"/>
+      <c r="Y240" s="112"/>
+      <c r="Z240" s="188"/>
+      <c r="AA240" s="188"/>
+      <c r="AB240" s="188"/>
+      <c r="AC240" s="188"/>
+      <c r="AD240" s="188"/>
+      <c r="AE240" s="188"/>
+      <c r="AF240" s="188"/>
+      <c r="AG240" s="188"/>
+      <c r="AH240" s="188"/>
+      <c r="AI240" s="188"/>
+    </row>
+    <row r="241" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B241" s="184"/>
+      <c r="C241" s="112"/>
+      <c r="D241" s="112"/>
+      <c r="E241" s="112"/>
+      <c r="F241" s="112"/>
+      <c r="G241" s="112"/>
+      <c r="H241" s="112"/>
+      <c r="I241" s="112"/>
+      <c r="J241" s="112"/>
+      <c r="K241" s="112"/>
+      <c r="L241" s="112"/>
+      <c r="M241" s="112"/>
+      <c r="N241" s="112"/>
+      <c r="O241" s="112"/>
+      <c r="P241" s="112"/>
+      <c r="Q241" s="112"/>
+      <c r="R241" s="112"/>
+      <c r="S241" s="112"/>
       <c r="T241" s="112"/>
       <c r="U241" s="112"/>
       <c r="V241" s="112"/>
       <c r="W241" s="112"/>
       <c r="X241" s="112"/>
-      <c r="Z241" s="101"/>
-    </row>
-    <row r="242" spans="1:26" customFormat="1" ht="16">
-      <c r="A242" s="101"/>
-      <c r="B242" s="101"/>
-      <c r="C242" s="101"/>
-      <c r="D242" s="101"/>
-      <c r="E242" s="101"/>
-      <c r="F242" s="101"/>
-      <c r="G242" s="101"/>
-      <c r="H242" s="101"/>
-      <c r="I242" s="101"/>
-      <c r="J242" s="101"/>
-      <c r="K242" s="101"/>
-      <c r="L242" s="101"/>
-      <c r="M242" s="101"/>
-      <c r="N242" s="101"/>
-      <c r="O242" s="101"/>
-      <c r="P242" s="101"/>
-      <c r="Q242" s="101"/>
-      <c r="R242" s="101"/>
-      <c r="S242" s="101"/>
+      <c r="Y241" s="112"/>
+      <c r="Z241" s="188"/>
+      <c r="AA241" s="188"/>
+      <c r="AB241" s="188"/>
+      <c r="AC241" s="188"/>
+      <c r="AD241" s="188"/>
+      <c r="AE241" s="188"/>
+      <c r="AF241" s="188"/>
+      <c r="AG241" s="188"/>
+      <c r="AH241" s="188"/>
+      <c r="AI241" s="188"/>
+    </row>
+    <row r="242" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B242" s="184"/>
+      <c r="C242" s="112"/>
+      <c r="D242" s="112"/>
+      <c r="E242" s="112"/>
+      <c r="F242" s="112"/>
+      <c r="G242" s="112"/>
+      <c r="H242" s="112"/>
+      <c r="I242" s="112"/>
+      <c r="J242" s="112"/>
+      <c r="K242" s="112"/>
+      <c r="L242" s="112"/>
+      <c r="M242" s="112"/>
+      <c r="N242" s="112"/>
+      <c r="O242" s="112"/>
+      <c r="P242" s="112"/>
+      <c r="Q242" s="112"/>
+      <c r="R242" s="112"/>
+      <c r="S242" s="112"/>
       <c r="T242" s="112"/>
       <c r="U242" s="112"/>
       <c r="V242" s="112"/>
       <c r="W242" s="112"/>
       <c r="X242" s="112"/>
-      <c r="Z242" s="101"/>
-    </row>
-    <row r="243" spans="1:26" customFormat="1" ht="16">
-      <c r="A243" s="101"/>
-      <c r="B243" s="101"/>
-      <c r="C243" s="101"/>
-      <c r="D243" s="101"/>
-      <c r="E243" s="101"/>
-      <c r="F243" s="101"/>
-      <c r="G243" s="101"/>
-      <c r="H243" s="101"/>
-      <c r="I243" s="101"/>
-      <c r="J243" s="101"/>
-      <c r="K243" s="101"/>
-      <c r="L243" s="101"/>
-      <c r="M243" s="101"/>
-      <c r="N243" s="101"/>
-      <c r="O243" s="101"/>
-      <c r="P243" s="101"/>
-      <c r="Q243" s="101"/>
-      <c r="R243" s="101"/>
-      <c r="S243" s="101"/>
-      <c r="T243" s="112"/>
-      <c r="U243" s="112"/>
-      <c r="V243" s="112"/>
-      <c r="W243" s="112"/>
-      <c r="X243" s="112"/>
-      <c r="Z243" s="101"/>
-    </row>
-    <row r="244" spans="1:26" customFormat="1" ht="16">
-      <c r="A244" s="101"/>
-      <c r="B244" s="101"/>
-      <c r="C244" s="101"/>
-      <c r="D244" s="101"/>
-      <c r="E244" s="101"/>
-      <c r="F244" s="101"/>
-      <c r="G244" s="101"/>
-      <c r="H244" s="101"/>
-      <c r="I244" s="101"/>
-      <c r="J244" s="101"/>
-      <c r="K244" s="101"/>
-      <c r="L244" s="101"/>
-      <c r="M244" s="101"/>
-      <c r="N244" s="101"/>
-      <c r="O244" s="101"/>
-      <c r="P244" s="101"/>
-      <c r="Q244" s="101"/>
-      <c r="R244" s="101"/>
-      <c r="S244" s="101"/>
-      <c r="T244" s="112"/>
-      <c r="U244" s="112"/>
-      <c r="V244" s="112"/>
-      <c r="W244" s="112"/>
-      <c r="X244" s="112"/>
-      <c r="Z244" s="101"/>
-    </row>
-    <row r="245" spans="1:26" customFormat="1" ht="16">
-      <c r="A245" s="101"/>
-      <c r="B245" s="101"/>
-      <c r="C245" s="101"/>
-      <c r="D245" s="101"/>
-      <c r="E245" s="101"/>
-      <c r="F245" s="101"/>
-      <c r="G245" s="101"/>
-      <c r="H245" s="101"/>
-      <c r="I245" s="101"/>
-      <c r="J245" s="101"/>
-      <c r="K245" s="101"/>
-      <c r="L245" s="101"/>
-      <c r="M245" s="101"/>
-      <c r="N245" s="101"/>
-      <c r="O245" s="101"/>
-      <c r="P245" s="101"/>
-      <c r="Q245" s="101"/>
-      <c r="R245" s="101"/>
-      <c r="S245" s="101"/>
-      <c r="Z245" s="101"/>
-    </row>
-    <row r="246" spans="1:26" customFormat="1" ht="16">
-      <c r="A246" s="101"/>
-      <c r="B246" s="101"/>
-      <c r="C246" s="101"/>
-      <c r="D246" s="101"/>
-      <c r="E246" s="101"/>
-      <c r="F246" s="101"/>
-      <c r="G246" s="101"/>
-      <c r="H246" s="101"/>
-      <c r="I246" s="101"/>
-      <c r="J246" s="101"/>
-      <c r="K246" s="101"/>
-      <c r="L246" s="101"/>
-      <c r="M246" s="101"/>
-      <c r="N246" s="101"/>
-      <c r="O246" s="101"/>
-      <c r="P246" s="101"/>
-      <c r="Q246" s="101"/>
-      <c r="R246" s="101"/>
-      <c r="S246" s="101"/>
-      <c r="Z246" s="101"/>
-    </row>
-    <row r="247" spans="1:26" customFormat="1" ht="16">
-      <c r="A247" s="101"/>
-      <c r="B247" s="101"/>
-      <c r="C247" s="101"/>
-      <c r="D247" s="101"/>
-      <c r="E247" s="101"/>
-      <c r="F247" s="101"/>
-      <c r="G247" s="101"/>
-      <c r="H247" s="101"/>
-      <c r="I247" s="101"/>
-      <c r="J247" s="101"/>
-      <c r="K247" s="101"/>
-      <c r="L247" s="101"/>
-      <c r="M247" s="101"/>
-      <c r="N247" s="101"/>
-      <c r="O247" s="101"/>
-      <c r="P247" s="101"/>
-      <c r="Q247" s="101"/>
-      <c r="R247" s="101"/>
-      <c r="S247" s="101"/>
-      <c r="Z247" s="101"/>
-    </row>
-    <row r="248" spans="1:26" customFormat="1" ht="16">
-      <c r="A248" s="101"/>
-      <c r="B248" s="101"/>
-      <c r="C248" s="101"/>
-      <c r="D248" s="101"/>
-      <c r="E248" s="101"/>
-      <c r="F248" s="101"/>
-      <c r="G248" s="101"/>
-      <c r="H248" s="101"/>
-      <c r="I248" s="101"/>
-      <c r="J248" s="101"/>
-      <c r="K248" s="101"/>
-      <c r="L248" s="101"/>
-      <c r="M248" s="101"/>
-      <c r="N248" s="101"/>
-      <c r="O248" s="101"/>
-      <c r="P248" s="101"/>
-      <c r="Q248" s="101"/>
-      <c r="R248" s="101"/>
-      <c r="S248" s="101"/>
-      <c r="Z248" s="101"/>
-    </row>
-    <row r="249" spans="1:26" customFormat="1" ht="16">
-      <c r="A249" s="102"/>
-      <c r="Z249" s="101"/>
-    </row>
-    <row r="250" spans="1:26" customFormat="1" ht="16">
-      <c r="A250" s="102"/>
-      <c r="Z250" s="101"/>
-    </row>
-    <row r="251" spans="1:26" customFormat="1" ht="16">
-      <c r="A251" s="102"/>
-      <c r="Z251" s="101"/>
-    </row>
-    <row r="252" spans="1:26" customFormat="1" ht="16">
-      <c r="A252" s="102"/>
-      <c r="Z252" s="101"/>
-    </row>
-    <row r="253" spans="1:26" customFormat="1" ht="16">
-      <c r="A253" s="102"/>
-      <c r="Z253" s="101"/>
-    </row>
-    <row r="254" spans="1:26" customFormat="1" ht="16">
-      <c r="A254" s="102"/>
-      <c r="Z254" s="101"/>
-    </row>
-    <row r="255" spans="1:26" customFormat="1" ht="16">
-      <c r="A255" s="102"/>
-      <c r="Z255" s="101"/>
-    </row>
-    <row r="256" spans="1:26" customFormat="1" ht="16">
-      <c r="A256" s="102"/>
-      <c r="Z256" s="101"/>
-    </row>
-    <row r="257" spans="1:26" customFormat="1" ht="16">
-      <c r="A257" s="102"/>
-      <c r="Z257" s="101"/>
-    </row>
-    <row r="258" spans="1:26" customFormat="1" ht="16">
-      <c r="A258" s="102"/>
-      <c r="Z258" s="101"/>
-    </row>
-    <row r="259" spans="1:26" customFormat="1" ht="16">
-      <c r="A259" s="102"/>
-      <c r="Z259" s="101"/>
-    </row>
-    <row r="260" spans="1:26" s="24" customFormat="1" ht="16">
-      <c r="A260" s="102"/>
-      <c r="B260"/>
-      <c r="C260"/>
-      <c r="D260"/>
-      <c r="E260"/>
-      <c r="F260"/>
-      <c r="G260"/>
-      <c r="H260"/>
-      <c r="I260"/>
-      <c r="J260"/>
-      <c r="K260"/>
-      <c r="L260"/>
-      <c r="M260"/>
-      <c r="N260"/>
-      <c r="O260"/>
-      <c r="P260"/>
-      <c r="Q260"/>
-      <c r="R260"/>
-      <c r="S260"/>
-      <c r="T260"/>
-      <c r="U260"/>
-      <c r="V260"/>
-      <c r="W260"/>
-      <c r="X260"/>
-      <c r="Y260"/>
-    </row>
-    <row r="261" spans="1:26" customFormat="1" ht="16">
-      <c r="A261" s="102"/>
-      <c r="Z261" s="101"/>
-    </row>
-    <row r="262" spans="1:26" customFormat="1" ht="16">
-      <c r="A262" s="102"/>
-      <c r="Z262" s="101"/>
-    </row>
-    <row r="263" spans="1:26" customFormat="1" ht="16">
+      <c r="Y242" s="112"/>
+      <c r="Z242" s="188"/>
+      <c r="AA242" s="188"/>
+      <c r="AB242" s="188"/>
+      <c r="AC242" s="188"/>
+      <c r="AD242" s="188"/>
+      <c r="AE242" s="188"/>
+      <c r="AF242" s="188"/>
+      <c r="AG242" s="188"/>
+      <c r="AH242" s="188"/>
+      <c r="AI242" s="188"/>
+    </row>
+    <row r="243" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B243" s="184"/>
+      <c r="C243" s="188"/>
+      <c r="D243" s="188"/>
+      <c r="E243" s="188"/>
+      <c r="F243" s="188"/>
+      <c r="G243" s="188"/>
+      <c r="H243" s="188"/>
+      <c r="I243" s="188"/>
+      <c r="J243" s="188"/>
+      <c r="K243" s="188"/>
+      <c r="L243" s="188"/>
+      <c r="M243" s="188"/>
+      <c r="N243" s="188"/>
+      <c r="O243" s="188"/>
+      <c r="P243" s="188"/>
+      <c r="Q243" s="188"/>
+      <c r="R243" s="188"/>
+      <c r="S243" s="188"/>
+      <c r="T243" s="188"/>
+      <c r="U243" s="188"/>
+      <c r="V243" s="188"/>
+      <c r="W243" s="188"/>
+      <c r="X243" s="188"/>
+      <c r="Y243" s="188"/>
+      <c r="Z243" s="188"/>
+      <c r="AA243" s="188"/>
+      <c r="AB243" s="188"/>
+      <c r="AC243" s="188"/>
+      <c r="AD243" s="188"/>
+      <c r="AE243" s="188"/>
+      <c r="AF243" s="188"/>
+      <c r="AG243" s="188"/>
+      <c r="AH243" s="188"/>
+      <c r="AI243" s="188"/>
+    </row>
+    <row r="244" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B244" s="184"/>
+      <c r="C244" s="188"/>
+      <c r="D244" s="188"/>
+      <c r="E244" s="188"/>
+      <c r="F244" s="188"/>
+      <c r="G244" s="188"/>
+      <c r="H244" s="188"/>
+      <c r="I244" s="188"/>
+      <c r="J244" s="188"/>
+      <c r="K244" s="188"/>
+      <c r="L244" s="188"/>
+      <c r="M244" s="188"/>
+      <c r="N244" s="188"/>
+      <c r="O244" s="188"/>
+      <c r="P244" s="188"/>
+      <c r="Q244" s="188"/>
+      <c r="R244" s="188"/>
+      <c r="S244" s="188"/>
+      <c r="T244" s="188"/>
+      <c r="U244" s="188"/>
+      <c r="V244" s="188"/>
+      <c r="W244" s="188"/>
+      <c r="X244" s="188"/>
+      <c r="Y244" s="188"/>
+      <c r="Z244" s="188"/>
+      <c r="AA244" s="188"/>
+      <c r="AB244" s="188"/>
+      <c r="AC244" s="188"/>
+      <c r="AD244" s="188"/>
+      <c r="AE244" s="188"/>
+      <c r="AF244" s="188"/>
+      <c r="AG244" s="188"/>
+      <c r="AH244" s="188"/>
+      <c r="AI244" s="188"/>
+    </row>
+    <row r="245" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B245" s="184"/>
+      <c r="C245" s="188"/>
+      <c r="D245" s="188"/>
+      <c r="E245" s="188"/>
+      <c r="F245" s="188"/>
+      <c r="G245" s="188"/>
+      <c r="H245" s="188"/>
+      <c r="I245" s="188"/>
+      <c r="J245" s="188"/>
+      <c r="K245" s="188"/>
+      <c r="L245" s="188"/>
+      <c r="M245" s="188"/>
+      <c r="N245" s="188"/>
+      <c r="O245" s="188"/>
+      <c r="P245" s="188"/>
+      <c r="Q245" s="188"/>
+      <c r="R245" s="188"/>
+      <c r="S245" s="188"/>
+      <c r="T245" s="188"/>
+      <c r="U245" s="188"/>
+      <c r="V245" s="188"/>
+      <c r="W245" s="188"/>
+      <c r="X245" s="188"/>
+      <c r="Y245" s="188"/>
+      <c r="Z245" s="188"/>
+      <c r="AA245" s="188"/>
+      <c r="AB245" s="188"/>
+      <c r="AC245" s="188"/>
+      <c r="AD245" s="188"/>
+      <c r="AE245" s="188"/>
+      <c r="AF245" s="188"/>
+      <c r="AG245" s="188"/>
+      <c r="AH245" s="188"/>
+      <c r="AI245" s="188"/>
+    </row>
+    <row r="246" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B246" s="184"/>
+      <c r="C246" s="188"/>
+      <c r="D246" s="188"/>
+      <c r="E246" s="188"/>
+      <c r="F246" s="188"/>
+      <c r="G246" s="188"/>
+      <c r="H246" s="188"/>
+      <c r="I246" s="188"/>
+      <c r="J246" s="188"/>
+      <c r="K246" s="188"/>
+      <c r="L246" s="188"/>
+      <c r="M246" s="188"/>
+      <c r="N246" s="188"/>
+      <c r="O246" s="188"/>
+      <c r="P246" s="188"/>
+      <c r="Q246" s="188"/>
+      <c r="R246" s="188"/>
+      <c r="S246" s="188"/>
+      <c r="T246" s="188"/>
+      <c r="U246" s="188"/>
+      <c r="V246" s="188"/>
+      <c r="W246" s="188"/>
+      <c r="X246" s="188"/>
+      <c r="Y246" s="188"/>
+      <c r="Z246" s="188"/>
+      <c r="AA246" s="188"/>
+      <c r="AB246" s="188"/>
+      <c r="AC246" s="188"/>
+      <c r="AD246" s="188"/>
+      <c r="AE246" s="188"/>
+      <c r="AF246" s="188"/>
+      <c r="AG246" s="188"/>
+      <c r="AH246" s="188"/>
+      <c r="AI246" s="188"/>
+    </row>
+    <row r="247" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B247" s="184"/>
+      <c r="C247" s="188"/>
+      <c r="D247" s="188"/>
+      <c r="E247" s="188"/>
+      <c r="F247" s="188"/>
+      <c r="G247" s="188"/>
+      <c r="H247" s="188"/>
+      <c r="I247" s="188"/>
+      <c r="J247" s="188"/>
+      <c r="K247" s="188"/>
+      <c r="L247" s="188"/>
+      <c r="M247" s="188"/>
+      <c r="N247" s="188"/>
+      <c r="O247" s="188"/>
+      <c r="P247" s="188"/>
+      <c r="Q247" s="188"/>
+      <c r="R247" s="188"/>
+      <c r="S247" s="188"/>
+      <c r="T247" s="188"/>
+      <c r="U247" s="188"/>
+      <c r="V247" s="188"/>
+      <c r="W247" s="188"/>
+      <c r="X247" s="188"/>
+      <c r="Y247" s="188"/>
+      <c r="Z247" s="188"/>
+      <c r="AA247" s="188"/>
+      <c r="AB247" s="188"/>
+      <c r="AC247" s="188"/>
+      <c r="AD247" s="188"/>
+      <c r="AE247" s="188"/>
+      <c r="AF247" s="188"/>
+      <c r="AG247" s="188"/>
+      <c r="AH247" s="188"/>
+      <c r="AI247" s="188"/>
+    </row>
+    <row r="248" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B248" s="184"/>
+      <c r="C248" s="188"/>
+      <c r="D248" s="188"/>
+      <c r="E248" s="188"/>
+      <c r="F248" s="188"/>
+      <c r="G248" s="188"/>
+      <c r="H248" s="188"/>
+      <c r="I248" s="188"/>
+      <c r="J248" s="188"/>
+      <c r="K248" s="188"/>
+      <c r="L248" s="188"/>
+      <c r="M248" s="188"/>
+      <c r="N248" s="188"/>
+      <c r="O248" s="188"/>
+      <c r="P248" s="188"/>
+      <c r="Q248" s="188"/>
+      <c r="R248" s="188"/>
+      <c r="S248" s="188"/>
+      <c r="T248" s="188"/>
+      <c r="U248" s="188"/>
+      <c r="V248" s="188"/>
+      <c r="W248" s="188"/>
+      <c r="X248" s="188"/>
+      <c r="Y248" s="188"/>
+      <c r="Z248" s="188"/>
+      <c r="AA248" s="188"/>
+      <c r="AB248" s="188"/>
+      <c r="AC248" s="188"/>
+      <c r="AD248" s="188"/>
+      <c r="AE248" s="188"/>
+      <c r="AF248" s="188"/>
+      <c r="AG248" s="188"/>
+      <c r="AH248" s="188"/>
+      <c r="AI248" s="188"/>
+    </row>
+    <row r="249" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B249" s="184"/>
+      <c r="C249" s="188"/>
+      <c r="D249" s="187">
+        <v>1.24</v>
+      </c>
+      <c r="E249" s="189"/>
+      <c r="F249" s="187"/>
+      <c r="G249" s="187">
+        <v>54600</v>
+      </c>
+      <c r="H249" s="187" t="s">
+        <v>187</v>
+      </c>
+      <c r="I249" s="187" t="s">
+        <v>189</v>
+      </c>
+      <c r="J249" s="188"/>
+      <c r="K249" s="188"/>
+      <c r="L249" s="188"/>
+      <c r="M249" s="188"/>
+      <c r="N249" s="188"/>
+      <c r="O249" s="188"/>
+      <c r="P249" s="188"/>
+      <c r="Q249" s="188"/>
+      <c r="R249" s="188"/>
+      <c r="S249" s="188"/>
+      <c r="T249" s="188"/>
+      <c r="U249" s="188"/>
+      <c r="V249" s="188"/>
+      <c r="W249" s="188"/>
+      <c r="X249" s="188"/>
+      <c r="Y249" s="188"/>
+      <c r="Z249" s="188"/>
+      <c r="AA249" s="188"/>
+      <c r="AB249" s="188"/>
+      <c r="AC249" s="188"/>
+      <c r="AD249" s="188"/>
+      <c r="AE249" s="188"/>
+      <c r="AF249" s="188"/>
+      <c r="AG249" s="188"/>
+      <c r="AH249" s="188"/>
+      <c r="AI249" s="188"/>
+    </row>
+    <row r="250" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B250" s="184"/>
+      <c r="C250" s="188"/>
+      <c r="D250" s="187"/>
+      <c r="E250" s="189"/>
+      <c r="F250" s="187"/>
+      <c r="G250" s="187">
+        <v>1000000</v>
+      </c>
+      <c r="H250" s="187" t="s">
+        <v>188</v>
+      </c>
+      <c r="I250" s="187"/>
+      <c r="J250" s="188"/>
+      <c r="K250" s="188"/>
+      <c r="L250" s="188"/>
+      <c r="M250" s="188"/>
+      <c r="N250" s="188"/>
+      <c r="O250" s="188"/>
+      <c r="P250" s="188"/>
+      <c r="Q250" s="188"/>
+      <c r="R250" s="188"/>
+      <c r="S250" s="188"/>
+      <c r="T250" s="188"/>
+      <c r="U250" s="188"/>
+      <c r="V250" s="188"/>
+      <c r="W250" s="188"/>
+      <c r="X250" s="188"/>
+      <c r="Y250" s="188"/>
+      <c r="Z250" s="188"/>
+      <c r="AA250" s="188"/>
+      <c r="AB250" s="188"/>
+      <c r="AC250" s="188"/>
+      <c r="AD250" s="188"/>
+      <c r="AE250" s="188"/>
+      <c r="AF250" s="188"/>
+      <c r="AG250" s="188"/>
+      <c r="AH250" s="188"/>
+      <c r="AI250" s="188"/>
+    </row>
+    <row r="251" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B251" s="184"/>
+      <c r="C251" s="188"/>
+      <c r="D251" s="187"/>
+      <c r="E251" s="189"/>
+      <c r="F251" s="187"/>
+      <c r="G251" s="187">
+        <v>5.4600000000000003E-2</v>
+      </c>
+      <c r="H251" s="187" t="s">
+        <v>187</v>
+      </c>
+      <c r="I251" s="187"/>
+      <c r="J251" s="188"/>
+      <c r="K251" s="188"/>
+      <c r="L251" s="188"/>
+      <c r="M251" s="188"/>
+      <c r="N251" s="188"/>
+      <c r="O251" s="188"/>
+      <c r="P251" s="188"/>
+      <c r="Q251" s="188"/>
+      <c r="R251" s="188"/>
+      <c r="S251" s="188"/>
+      <c r="T251" s="188"/>
+      <c r="U251" s="188"/>
+      <c r="V251" s="188"/>
+      <c r="W251" s="188"/>
+      <c r="X251" s="188"/>
+      <c r="Y251" s="188"/>
+      <c r="Z251" s="188"/>
+      <c r="AA251" s="188"/>
+      <c r="AB251" s="188"/>
+      <c r="AC251" s="188"/>
+      <c r="AD251" s="188"/>
+      <c r="AE251" s="188"/>
+      <c r="AF251" s="188"/>
+      <c r="AG251" s="188"/>
+      <c r="AH251" s="188"/>
+      <c r="AI251" s="188"/>
+    </row>
+    <row r="252" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B252" s="184"/>
+      <c r="C252" s="188"/>
+      <c r="D252" s="188"/>
+      <c r="E252" s="188"/>
+      <c r="F252" s="188"/>
+      <c r="G252" s="188"/>
+      <c r="H252" s="188"/>
+      <c r="I252" s="188"/>
+      <c r="J252" s="188"/>
+      <c r="K252" s="188"/>
+      <c r="L252" s="188"/>
+      <c r="M252" s="188"/>
+      <c r="N252" s="188"/>
+      <c r="O252" s="188"/>
+      <c r="P252" s="188"/>
+      <c r="Q252" s="188"/>
+      <c r="R252" s="188"/>
+      <c r="S252" s="188"/>
+      <c r="T252" s="188"/>
+      <c r="U252" s="188"/>
+      <c r="V252" s="188"/>
+      <c r="W252" s="188"/>
+      <c r="X252" s="188"/>
+      <c r="Y252" s="188"/>
+      <c r="Z252" s="188"/>
+      <c r="AA252" s="188"/>
+      <c r="AB252" s="188"/>
+      <c r="AC252" s="188"/>
+      <c r="AD252" s="188"/>
+      <c r="AE252" s="188"/>
+      <c r="AF252" s="188"/>
+      <c r="AG252" s="188"/>
+      <c r="AH252" s="188"/>
+      <c r="AI252" s="188"/>
+    </row>
+    <row r="253" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B253" s="184"/>
+      <c r="C253" s="188"/>
+      <c r="D253" s="188"/>
+      <c r="E253" s="188"/>
+      <c r="F253" s="188"/>
+      <c r="G253" s="188"/>
+      <c r="H253" s="188"/>
+      <c r="I253" s="188"/>
+      <c r="J253" s="188"/>
+      <c r="K253" s="188"/>
+      <c r="L253" s="188"/>
+      <c r="M253" s="188"/>
+      <c r="N253" s="188"/>
+      <c r="O253" s="188"/>
+      <c r="P253" s="188"/>
+      <c r="Q253" s="188"/>
+      <c r="R253" s="188"/>
+      <c r="S253" s="188"/>
+      <c r="T253" s="188"/>
+      <c r="U253" s="188"/>
+      <c r="V253" s="188"/>
+      <c r="W253" s="188"/>
+      <c r="X253" s="188"/>
+      <c r="Y253" s="188"/>
+      <c r="Z253" s="188"/>
+      <c r="AA253" s="188"/>
+      <c r="AB253" s="188"/>
+      <c r="AC253" s="188"/>
+      <c r="AD253" s="188"/>
+      <c r="AE253" s="188"/>
+      <c r="AF253" s="188"/>
+      <c r="AG253" s="188"/>
+      <c r="AH253" s="188"/>
+      <c r="AI253" s="188"/>
+    </row>
+    <row r="254" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B254" s="184"/>
+      <c r="C254" s="188"/>
+      <c r="D254" s="188"/>
+      <c r="E254" s="188"/>
+      <c r="F254" s="188"/>
+      <c r="G254" s="188"/>
+      <c r="H254" s="188"/>
+      <c r="I254" s="188"/>
+      <c r="J254" s="188"/>
+      <c r="K254" s="188"/>
+      <c r="L254" s="188"/>
+      <c r="M254" s="188"/>
+      <c r="N254" s="188"/>
+      <c r="O254" s="188"/>
+      <c r="P254" s="188"/>
+      <c r="Q254" s="188"/>
+      <c r="R254" s="188"/>
+      <c r="S254" s="188"/>
+      <c r="T254" s="188"/>
+      <c r="U254" s="188"/>
+      <c r="V254" s="188"/>
+      <c r="W254" s="188"/>
+      <c r="X254" s="188"/>
+      <c r="Y254" s="188"/>
+      <c r="Z254" s="188"/>
+      <c r="AA254" s="188"/>
+      <c r="AB254" s="188"/>
+      <c r="AC254" s="188"/>
+      <c r="AD254" s="188"/>
+      <c r="AE254" s="188"/>
+      <c r="AF254" s="188"/>
+      <c r="AG254" s="188"/>
+      <c r="AH254" s="188"/>
+      <c r="AI254" s="188"/>
+    </row>
+    <row r="255" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B255" s="184"/>
+      <c r="C255" s="188"/>
+      <c r="D255" s="188"/>
+      <c r="E255" s="188"/>
+      <c r="F255" s="188"/>
+      <c r="G255" s="188"/>
+      <c r="H255" s="188"/>
+      <c r="I255" s="188"/>
+      <c r="J255" s="188"/>
+      <c r="K255" s="188"/>
+      <c r="L255" s="188"/>
+      <c r="M255" s="188"/>
+      <c r="N255" s="188"/>
+      <c r="O255" s="188"/>
+      <c r="P255" s="188"/>
+      <c r="Q255" s="188"/>
+      <c r="R255" s="188"/>
+      <c r="S255" s="188"/>
+      <c r="T255" s="188"/>
+      <c r="U255" s="188"/>
+      <c r="V255" s="188"/>
+      <c r="W255" s="188"/>
+      <c r="X255" s="188"/>
+      <c r="Y255" s="188"/>
+      <c r="Z255" s="188"/>
+      <c r="AA255" s="188"/>
+      <c r="AB255" s="188"/>
+      <c r="AC255" s="188"/>
+      <c r="AD255" s="188"/>
+      <c r="AE255" s="188"/>
+      <c r="AF255" s="188"/>
+      <c r="AG255" s="188"/>
+      <c r="AH255" s="188"/>
+      <c r="AI255" s="188"/>
+    </row>
+    <row r="256" spans="2:35" s="181" customFormat="1" ht="16">
+      <c r="B256" s="184"/>
+      <c r="C256" s="188"/>
+      <c r="D256" s="188"/>
+      <c r="E256" s="188"/>
+      <c r="F256" s="188"/>
+      <c r="G256" s="188"/>
+      <c r="H256" s="188"/>
+      <c r="I256" s="188"/>
+      <c r="J256" s="188"/>
+      <c r="K256" s="188"/>
+      <c r="L256" s="188"/>
+      <c r="M256" s="188"/>
+      <c r="N256" s="188"/>
+      <c r="O256" s="188"/>
+      <c r="P256" s="188"/>
+      <c r="Q256" s="188"/>
+      <c r="R256" s="188"/>
+      <c r="S256" s="188"/>
+      <c r="T256" s="188"/>
+      <c r="U256" s="188"/>
+      <c r="V256" s="188"/>
+      <c r="W256" s="188"/>
+      <c r="X256" s="188"/>
+      <c r="Y256" s="188"/>
+      <c r="Z256" s="188"/>
+      <c r="AA256" s="188"/>
+      <c r="AB256" s="188"/>
+      <c r="AC256" s="188"/>
+      <c r="AD256" s="188"/>
+      <c r="AE256" s="188"/>
+      <c r="AF256" s="188"/>
+      <c r="AG256" s="188"/>
+      <c r="AH256" s="188"/>
+      <c r="AI256" s="188"/>
+    </row>
+    <row r="257" spans="1:35" s="181" customFormat="1" ht="16">
+      <c r="B257" s="184"/>
+      <c r="C257" s="188"/>
+      <c r="D257" s="188"/>
+      <c r="E257" s="188"/>
+      <c r="F257" s="188"/>
+      <c r="G257" s="188"/>
+      <c r="H257" s="188"/>
+      <c r="I257" s="188"/>
+      <c r="J257" s="188"/>
+      <c r="K257" s="188"/>
+      <c r="L257" s="188"/>
+      <c r="M257" s="188"/>
+      <c r="N257" s="188"/>
+      <c r="O257" s="188"/>
+      <c r="P257" s="188"/>
+      <c r="Q257" s="188"/>
+      <c r="R257" s="188"/>
+      <c r="S257" s="188"/>
+      <c r="T257" s="188"/>
+      <c r="U257" s="188"/>
+      <c r="V257" s="188"/>
+      <c r="W257" s="188"/>
+      <c r="X257" s="188"/>
+      <c r="Y257" s="188"/>
+      <c r="Z257" s="188"/>
+      <c r="AA257" s="188"/>
+      <c r="AB257" s="188"/>
+      <c r="AC257" s="188"/>
+      <c r="AD257" s="188"/>
+      <c r="AE257" s="188"/>
+      <c r="AF257" s="188"/>
+      <c r="AG257" s="188"/>
+      <c r="AH257" s="188"/>
+      <c r="AI257" s="188"/>
+    </row>
+    <row r="258" spans="1:35" s="181" customFormat="1" ht="16">
+      <c r="B258" s="184"/>
+      <c r="C258" s="188"/>
+      <c r="D258" s="188"/>
+      <c r="E258" s="188"/>
+      <c r="F258" s="188"/>
+      <c r="G258" s="188"/>
+      <c r="H258" s="188"/>
+      <c r="I258" s="188"/>
+      <c r="J258" s="188"/>
+      <c r="K258" s="188"/>
+      <c r="L258" s="188"/>
+      <c r="M258" s="188"/>
+      <c r="N258" s="188"/>
+      <c r="O258" s="188"/>
+      <c r="P258" s="188"/>
+      <c r="Q258" s="188"/>
+      <c r="R258" s="188"/>
+      <c r="S258" s="188"/>
+      <c r="T258" s="188"/>
+      <c r="U258" s="188"/>
+      <c r="V258" s="188"/>
+      <c r="W258" s="188"/>
+      <c r="X258" s="188"/>
+      <c r="Y258" s="188"/>
+      <c r="Z258" s="188"/>
+      <c r="AA258" s="188"/>
+      <c r="AB258" s="188"/>
+      <c r="AC258" s="188"/>
+      <c r="AD258" s="188"/>
+      <c r="AE258" s="188"/>
+      <c r="AF258" s="188"/>
+      <c r="AG258" s="188"/>
+      <c r="AH258" s="188"/>
+      <c r="AI258" s="188"/>
+    </row>
+    <row r="259" spans="1:35" s="181" customFormat="1" ht="16">
+      <c r="B259" s="184"/>
+      <c r="C259" s="188"/>
+      <c r="D259" s="188"/>
+      <c r="E259" s="188"/>
+      <c r="F259" s="188"/>
+      <c r="G259" s="188"/>
+      <c r="H259" s="188"/>
+      <c r="I259" s="188"/>
+      <c r="J259" s="188"/>
+      <c r="K259" s="188"/>
+      <c r="L259" s="188"/>
+      <c r="M259" s="188"/>
+      <c r="N259" s="188"/>
+      <c r="O259" s="188"/>
+      <c r="P259" s="188"/>
+      <c r="Q259" s="188"/>
+      <c r="R259" s="188"/>
+      <c r="S259" s="188"/>
+      <c r="T259" s="188"/>
+      <c r="U259" s="188"/>
+      <c r="V259" s="188"/>
+      <c r="W259" s="188"/>
+      <c r="X259" s="188"/>
+      <c r="Y259" s="188"/>
+      <c r="Z259" s="188"/>
+      <c r="AA259" s="188"/>
+      <c r="AB259" s="188"/>
+      <c r="AC259" s="188"/>
+      <c r="AD259" s="188"/>
+      <c r="AE259" s="188"/>
+      <c r="AF259" s="188"/>
+      <c r="AG259" s="188"/>
+      <c r="AH259" s="188"/>
+      <c r="AI259" s="188"/>
+    </row>
+    <row r="260" spans="1:35" s="181" customFormat="1" ht="16">
+      <c r="B260" s="184"/>
+      <c r="C260" s="188"/>
+      <c r="D260" s="188"/>
+      <c r="E260" s="188"/>
+      <c r="F260" s="188"/>
+      <c r="G260" s="188"/>
+      <c r="H260" s="188"/>
+      <c r="I260" s="188"/>
+      <c r="J260" s="188"/>
+      <c r="K260" s="188"/>
+      <c r="L260" s="188"/>
+      <c r="M260" s="188"/>
+      <c r="N260" s="188"/>
+      <c r="O260" s="188"/>
+      <c r="P260" s="188"/>
+      <c r="Q260" s="188"/>
+      <c r="R260" s="188"/>
+      <c r="S260" s="188"/>
+      <c r="T260" s="188"/>
+      <c r="U260" s="188"/>
+      <c r="V260" s="188"/>
+      <c r="W260" s="188"/>
+      <c r="X260" s="188"/>
+      <c r="Y260" s="188"/>
+      <c r="Z260" s="188"/>
+      <c r="AA260" s="188"/>
+      <c r="AB260" s="188"/>
+      <c r="AC260" s="188"/>
+      <c r="AD260" s="188"/>
+      <c r="AE260" s="188"/>
+      <c r="AF260" s="188"/>
+      <c r="AG260" s="188"/>
+      <c r="AH260" s="188"/>
+      <c r="AI260" s="188"/>
+    </row>
+    <row r="261" spans="1:35" s="181" customFormat="1" ht="16">
+      <c r="B261" s="184"/>
+      <c r="C261" s="188"/>
+      <c r="D261" s="188"/>
+      <c r="E261" s="188"/>
+      <c r="F261" s="188"/>
+      <c r="G261" s="188"/>
+      <c r="H261" s="188"/>
+      <c r="I261" s="188"/>
+      <c r="J261" s="188"/>
+      <c r="K261" s="188"/>
+      <c r="L261" s="188"/>
+      <c r="M261" s="188"/>
+      <c r="N261" s="188"/>
+      <c r="O261" s="188"/>
+      <c r="P261" s="188"/>
+      <c r="Q261" s="188"/>
+      <c r="R261" s="188"/>
+      <c r="S261" s="188"/>
+      <c r="T261" s="188"/>
+      <c r="U261" s="188"/>
+      <c r="V261" s="188"/>
+      <c r="W261" s="188"/>
+      <c r="X261" s="188"/>
+      <c r="Y261" s="188"/>
+      <c r="Z261" s="188"/>
+      <c r="AA261" s="188"/>
+      <c r="AB261" s="188"/>
+      <c r="AC261" s="188"/>
+      <c r="AD261" s="188"/>
+      <c r="AE261" s="188"/>
+      <c r="AF261" s="188"/>
+      <c r="AG261" s="188"/>
+      <c r="AH261" s="188"/>
+      <c r="AI261" s="188"/>
+    </row>
+    <row r="262" spans="1:35" s="181" customFormat="1" ht="16">
+      <c r="B262" s="184"/>
+      <c r="C262" s="188"/>
+      <c r="D262" s="188"/>
+      <c r="E262" s="188"/>
+      <c r="F262" s="188"/>
+      <c r="G262" s="188"/>
+      <c r="H262" s="188"/>
+      <c r="I262" s="188"/>
+      <c r="J262" s="188"/>
+      <c r="K262" s="188"/>
+      <c r="L262" s="188"/>
+      <c r="M262" s="188"/>
+      <c r="N262" s="188"/>
+      <c r="O262" s="188"/>
+      <c r="P262" s="188"/>
+      <c r="Q262" s="188"/>
+      <c r="R262" s="188"/>
+      <c r="S262" s="188"/>
+      <c r="T262" s="188"/>
+      <c r="U262" s="188"/>
+      <c r="V262" s="188"/>
+      <c r="W262" s="188"/>
+      <c r="X262" s="188"/>
+      <c r="Y262" s="188"/>
+      <c r="Z262" s="188"/>
+      <c r="AA262" s="188"/>
+      <c r="AB262" s="188"/>
+      <c r="AC262" s="188"/>
+      <c r="AD262" s="188"/>
+      <c r="AE262" s="188"/>
+      <c r="AF262" s="188"/>
+      <c r="AG262" s="188"/>
+      <c r="AH262" s="188"/>
+      <c r="AI262" s="188"/>
+    </row>
+    <row r="263" spans="1:35" customFormat="1" ht="16">
       <c r="A263" s="102"/>
       <c r="Z263" s="101"/>
     </row>
-    <row r="264" spans="1:26" customFormat="1" ht="16">
+    <row r="264" spans="1:35" customFormat="1" ht="16">
       <c r="A264" s="102"/>
       <c r="Z264" s="101"/>
     </row>
-    <row r="265" spans="1:26" customFormat="1" ht="16">
+    <row r="265" spans="1:35" customFormat="1" ht="16">
       <c r="A265" s="102"/>
       <c r="Z265" s="101"/>
     </row>
-    <row r="266" spans="1:26" customFormat="1" ht="16">
+    <row r="266" spans="1:35" customFormat="1" ht="16">
       <c r="A266" s="102"/>
       <c r="Z266" s="101"/>
     </row>
-    <row r="267" spans="1:26" customFormat="1" ht="16">
+    <row r="267" spans="1:35" customFormat="1" ht="16">
       <c r="A267" s="102"/>
       <c r="Z267" s="101"/>
     </row>
-    <row r="268" spans="1:26" customFormat="1" ht="16">
+    <row r="268" spans="1:35" customFormat="1" ht="16">
       <c r="A268" s="102"/>
       <c r="Z268" s="101"/>
     </row>
-    <row r="269" spans="1:26" customFormat="1" ht="16">
+    <row r="269" spans="1:35" customFormat="1" ht="16">
       <c r="A269" s="102"/>
       <c r="Z269" s="101"/>
     </row>
-    <row r="270" spans="1:26" customFormat="1" ht="16">
+    <row r="270" spans="1:35" customFormat="1" ht="16">
       <c r="A270" s="102"/>
       <c r="Z270" s="101"/>
     </row>
-    <row r="271" spans="1:26" customFormat="1" ht="16">
+    <row r="271" spans="1:35" customFormat="1" ht="16">
       <c r="A271" s="102"/>
       <c r="Z271" s="101"/>
     </row>
-    <row r="272" spans="1:26" customFormat="1" ht="16">
+    <row r="272" spans="1:35" customFormat="1" ht="16">
       <c r="A272" s="102"/>
       <c r="Z272" s="101"/>
     </row>

</xml_diff>